<commit_message>
Change the common names to Arabic names
</commit_message>
<xml_diff>
--- a/data/Outdoor plants.xlsx
+++ b/data/Outdoor plants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\landscapingUOB-api\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A288B144-6182-4FDF-9CA0-2755D5B18223}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D251AA8-28D4-410D-A5C4-C833767C13D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{8B519764-563C-4CD5-B8E9-9B8B0702B21B}"/>
   </bookViews>
@@ -1936,7 +1936,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F43C3B61-471E-4868-9D01-BC7FF88A37C8}">
   <dimension ref="A1:U186"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
     </sheetView>
@@ -6750,6 +6750,14 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="7855343b-5261-4afc-a17c-d4c130fbaa85" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000D89A625C5B6364BB7302BED22ED65DA" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="05bac8ad6e033965382d52c38353e541">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="7855343b-5261-4afc-a17c-d4c130fbaa85" xmlns:ns4="72f917e0-5d36-43ac-975d-26afa4cf7fc0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="452e5605b09f318b6d66379e79837bd5" ns3:_="" ns4:_="">
     <xsd:import namespace="7855343b-5261-4afc-a17c-d4c130fbaa85"/>
@@ -6996,14 +7004,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="7855343b-5261-4afc-a17c-d4c130fbaa85" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BE4A15A-EC2D-4537-B6DC-2F235DBE6314}">
   <ds:schemaRefs>
@@ -7013,6 +7013,16 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F53F9CFB-0E7D-4BF1-9CBE-0D133C6536E4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="7855343b-5261-4afc-a17c-d4c130fbaa85"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56978299-3DC6-451D-A1E5-57FB07C431CC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7029,14 +7039,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F53F9CFB-0E7D-4BF1-9CBE-0D133C6536E4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="7855343b-5261-4afc-a17c-d4c130fbaa85"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
3 more plants added with several plants' image modifications
</commit_message>
<xml_diff>
--- a/data/Outdoor plants.xlsx
+++ b/data/Outdoor plants.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\landscapingUOB-api\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F3195EB9-01E0-43BA-AE45-18A067FF6FC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FFCC3F4-78AE-4719-87AB-773A0AAF169F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{8B519764-563C-4CD5-B8E9-9B8B0702B21B}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1244" uniqueCount="470">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1304" uniqueCount="491">
   <si>
     <t>Plant ID</t>
   </si>
@@ -967,12 +967,6 @@
     <t>Conocarpus erectus</t>
   </si>
   <si>
-    <t>كونوكاربس</t>
-  </si>
-  <si>
-    <t>https://i.postimg.cc/MHC3GCcR/Conocarpus-erectus-2.jpg</t>
-  </si>
-  <si>
     <t>1 - 20 m</t>
   </si>
   <si>
@@ -1012,12 +1006,6 @@
     <t>Ocimum basilicum</t>
   </si>
   <si>
-    <t>المشموم</t>
-  </si>
-  <si>
-    <t>https://i.postimg.cc/Xq6ZLkNk/pexels-brent-keane-181485-1684990.jpg</t>
-  </si>
-  <si>
     <t>0.3 - 0.5 m</t>
   </si>
   <si>
@@ -1451,13 +1439,88 @@
   </si>
   <si>
     <t>Gate 3-S55</t>
+  </si>
+  <si>
+    <t>المشموم البحريني</t>
+  </si>
+  <si>
+    <t>دمس رمادي</t>
+  </si>
+  <si>
+    <t>https://i.postimg.cc/5y0VwZzt/almshmwm-albhryny.jpg</t>
+  </si>
+  <si>
+    <t>https://i.postimg.cc/pX3HFcLL/dms-rmady.jpg</t>
+  </si>
+  <si>
+    <t>OP-059</t>
+  </si>
+  <si>
+    <t>OP-060</t>
+  </si>
+  <si>
+    <t>Euphorbia tithymaloides</t>
+  </si>
+  <si>
+    <t>1.5 - 2.5 m</t>
+  </si>
+  <si>
+    <t>15-25 g/year</t>
+  </si>
+  <si>
+    <t>30-50 g/year</t>
+  </si>
+  <si>
+    <t>Crinum asiaticum</t>
+  </si>
+  <si>
+    <t>0.6 - 1.0 m</t>
+  </si>
+  <si>
+    <t>20-35 g/year</t>
+  </si>
+  <si>
+    <t>40-70 g/year</t>
+  </si>
+  <si>
+    <t>OP-061</t>
+  </si>
+  <si>
+    <t>Volkameria inermis</t>
+  </si>
+  <si>
+    <t>2.0 - 4.0 m</t>
+  </si>
+  <si>
+    <t>1.5 - 3.0 m</t>
+  </si>
+  <si>
+    <t>60-100 g/year</t>
+  </si>
+  <si>
+    <t>الفربيون تيثيمالويدس</t>
+  </si>
+  <si>
+    <t>زنبق العنكبوت</t>
+  </si>
+  <si>
+    <t>الياسمين الزفر</t>
+  </si>
+  <si>
+    <t>https://i.postimg.cc/JnQT10GQ/alfrbywn-tythymalwyds.jpg</t>
+  </si>
+  <si>
+    <t>https://i.postimg.cc/ZRLfTnCV/alyasmyn-alzfr.jpg</t>
+  </si>
+  <si>
+    <t>https://i.postimg.cc/Kz59ZjRN/znbq-alʿnkbwt.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1534,11 +1597,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1588,9 +1652,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
+    <cellStyle name="Hyperlink 2" xfId="2" xr:uid="{AE659222-7167-453C-8DC0-4FDDEB47B12A}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -1937,36 +2009,36 @@
   <dimension ref="A1:U186"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C48" sqref="C48"/>
+      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E64" sqref="E64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="4"/>
-    <col min="2" max="2" width="32.42578125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="23.140625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="47.85546875" style="4" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" style="4" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.140625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" style="4" customWidth="1"/>
-    <col min="11" max="11" width="14.5703125" style="4" customWidth="1"/>
-    <col min="12" max="13" width="9.140625" style="4"/>
-    <col min="14" max="14" width="14.140625" style="4" customWidth="1"/>
-    <col min="15" max="15" width="11.7109375" style="4" customWidth="1"/>
-    <col min="16" max="16" width="16.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="21.140625" style="4" customWidth="1"/>
-    <col min="20" max="20" width="27.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="33.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="9.1796875" style="4"/>
+    <col min="2" max="2" width="32.453125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="23.1796875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="12.453125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="47.81640625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="17.7265625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="15.26953125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="16.81640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.1796875" style="4" customWidth="1"/>
+    <col min="10" max="10" width="12.453125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="14.54296875" style="4" customWidth="1"/>
+    <col min="12" max="13" width="9.1796875" style="4"/>
+    <col min="14" max="14" width="14.1796875" style="4" customWidth="1"/>
+    <col min="15" max="15" width="11.7265625" style="4" customWidth="1"/>
+    <col min="16" max="16" width="16.26953125" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.453125" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.7265625" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21.1796875" style="4" customWidth="1"/>
+    <col min="20" max="20" width="27.26953125" style="4" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="33.7265625" style="4" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="9.1796875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="14.45">
+    <row r="1" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2031,7 +2103,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="14.45">
+    <row r="2" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>21</v>
       </c>
@@ -2096,7 +2168,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="15.75">
+    <row r="3" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>37</v>
       </c>
@@ -2161,7 +2233,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="14.45">
+    <row r="4" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>49</v>
       </c>
@@ -2226,7 +2298,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="14.45">
+    <row r="5" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>58</v>
       </c>
@@ -2291,7 +2363,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="14.45">
+    <row r="6" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>66</v>
       </c>
@@ -2356,7 +2428,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="14.45">
+    <row r="7" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>75</v>
       </c>
@@ -2421,7 +2493,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="14.45">
+    <row r="8" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>82</v>
       </c>
@@ -2486,7 +2558,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="14.45">
+    <row r="9" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>92</v>
       </c>
@@ -2551,7 +2623,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="14.45">
+    <row r="10" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>97</v>
       </c>
@@ -2616,7 +2688,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="14.45">
+    <row r="11" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>104</v>
       </c>
@@ -2681,7 +2753,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="14.45">
+    <row r="12" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>111</v>
       </c>
@@ -2746,7 +2818,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="14.45">
+    <row r="13" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>115</v>
       </c>
@@ -2811,7 +2883,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="14.45">
+    <row r="14" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>122</v>
       </c>
@@ -2876,7 +2948,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="14.45">
+    <row r="15" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>129</v>
       </c>
@@ -2941,7 +3013,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="14.45">
+    <row r="16" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>136</v>
       </c>
@@ -3006,7 +3078,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="17" spans="1:21" ht="14.45">
+    <row r="17" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>143</v>
       </c>
@@ -3071,7 +3143,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="18" spans="1:21" ht="14.45">
+    <row r="18" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>150</v>
       </c>
@@ -3136,7 +3208,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="19" spans="1:21" ht="14.45">
+    <row r="19" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
         <v>159</v>
       </c>
@@ -3201,7 +3273,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="20" spans="1:21" ht="14.45">
+    <row r="20" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>167</v>
       </c>
@@ -3266,7 +3338,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="21" spans="1:21" ht="14.45">
+    <row r="21" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
         <v>175</v>
       </c>
@@ -3331,7 +3403,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="22" spans="1:21" ht="14.45">
+    <row r="22" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
         <v>183</v>
       </c>
@@ -3396,7 +3468,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="15.75">
+    <row r="23" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
         <v>192</v>
       </c>
@@ -3461,7 +3533,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="24" spans="1:21" ht="14.45">
+    <row r="24" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
         <v>198</v>
       </c>
@@ -3526,7 +3598,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="25" spans="1:21" ht="14.45">
+    <row r="25" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
         <v>206</v>
       </c>
@@ -3591,7 +3663,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="26" spans="1:21" ht="14.45">
+    <row r="26" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
         <v>214</v>
       </c>
@@ -3656,7 +3728,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="27" spans="1:21" ht="14.45">
+    <row r="27" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
         <v>221</v>
       </c>
@@ -3721,7 +3793,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="28" spans="1:21" ht="14.45">
+    <row r="28" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="s">
         <v>228</v>
       </c>
@@ -3786,7 +3858,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="29" spans="1:21" ht="14.45">
+    <row r="29" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="s">
         <v>236</v>
       </c>
@@ -3851,7 +3923,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="30" spans="1:21" ht="14.45">
+    <row r="30" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
         <v>242</v>
       </c>
@@ -3916,7 +3988,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="31" spans="1:21" ht="14.45">
+    <row r="31" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
         <v>250</v>
       </c>
@@ -3981,7 +4053,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="32" spans="1:21" ht="15.75" customHeight="1">
+    <row r="32" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="s">
         <v>257</v>
       </c>
@@ -4046,7 +4118,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="33" spans="1:21" ht="14.45">
+    <row r="33" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A33" s="4" t="s">
         <v>265</v>
       </c>
@@ -4111,7 +4183,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="34" spans="1:21" ht="14.45">
+    <row r="34" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A34" s="4" t="s">
         <v>271</v>
       </c>
@@ -4176,7 +4248,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="35" spans="1:21" ht="14.45">
+    <row r="35" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
         <v>277</v>
       </c>
@@ -4241,7 +4313,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="36" spans="1:21" ht="14.45">
+    <row r="36" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A36" s="4" t="s">
         <v>283</v>
       </c>
@@ -4306,7 +4378,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="37" spans="1:21" ht="14.45">
+    <row r="37" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A37" s="4" t="s">
         <v>290</v>
       </c>
@@ -4371,7 +4443,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="38" spans="1:21" ht="14.45">
+    <row r="38" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A38" s="4" t="s">
         <v>295</v>
       </c>
@@ -4436,7 +4508,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="39" spans="1:21" ht="14.45">
+    <row r="39" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A39" s="4" t="s">
         <v>301</v>
       </c>
@@ -4501,7 +4573,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="40" spans="1:21" ht="14.45">
+    <row r="40" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A40" s="4" t="s">
         <v>306</v>
       </c>
@@ -4509,13 +4581,13 @@
         <v>307</v>
       </c>
       <c r="C40" s="24" t="s">
-        <v>308</v>
+        <v>467</v>
       </c>
       <c r="D40" s="13" t="s">
         <v>24</v>
       </c>
       <c r="E40" s="13" t="s">
-        <v>309</v>
+        <v>469</v>
       </c>
       <c r="F40" s="8" t="s">
         <v>154</v>
@@ -4530,7 +4602,7 @@
         <v>53</v>
       </c>
       <c r="J40" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="K40" s="8" t="s">
         <v>232</v>
@@ -4560,27 +4632,27 @@
         <v>32</v>
       </c>
       <c r="T40" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="U40" s="4" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A41" s="4" t="s">
         <v>311</v>
       </c>
-      <c r="U40" s="4" t="s">
+      <c r="B41" s="4" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="41" spans="1:21" ht="14.45">
-      <c r="A41" s="4" t="s">
+      <c r="C41" s="24" t="s">
         <v>313</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>314</v>
-      </c>
-      <c r="C41" s="24" t="s">
-        <v>315</v>
       </c>
       <c r="D41" s="6" t="s">
         <v>24</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="F41" s="4" t="s">
         <v>70</v>
@@ -4595,10 +4667,10 @@
         <v>53</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="K41" s="4" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="L41" s="4" t="s">
         <v>33</v>
@@ -4625,27 +4697,27 @@
         <v>32</v>
       </c>
       <c r="T41" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="U41" s="4" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A42" s="4" t="s">
         <v>319</v>
       </c>
-      <c r="U41" s="4" t="s">
+      <c r="B42" s="4" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="42" spans="1:21" ht="14.45">
-      <c r="A42" s="4" t="s">
-        <v>321</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>322</v>
-      </c>
       <c r="C42" s="24" t="s">
-        <v>323</v>
+        <v>466</v>
       </c>
       <c r="D42" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E42" s="6" t="s">
-        <v>324</v>
+      <c r="E42" s="12" t="s">
+        <v>468</v>
       </c>
       <c r="F42" s="4" t="s">
         <v>26</v>
@@ -4663,7 +4735,7 @@
         <v>89</v>
       </c>
       <c r="K42" s="4" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="L42" s="4" t="s">
         <v>31</v>
@@ -4690,30 +4762,30 @@
         <v>32</v>
       </c>
       <c r="T42" s="4" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="U42" s="4" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="43" spans="1:21" ht="14.45">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A43" s="4" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="C43" s="24" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="D43" s="6" t="s">
         <v>24</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="G43" s="4" t="s">
         <v>42</v>
@@ -4755,27 +4827,27 @@
         <v>32</v>
       </c>
       <c r="T43" s="4" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="U43" s="4" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="44" spans="1:21" ht="14.45">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A44" s="4" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="C44" s="24" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="D44" s="15" t="s">
         <v>24</v>
       </c>
       <c r="E44" s="15" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="F44" s="4" t="s">
         <v>26</v>
@@ -4820,30 +4892,30 @@
         <v>28</v>
       </c>
       <c r="T44" s="4" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="U44" s="4" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="45" spans="1:21" ht="15.75">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A45" s="4" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="C45" s="24" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="D45" s="12" t="s">
         <v>24</v>
       </c>
       <c r="E45" s="12" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="G45" s="4" t="s">
         <v>87</v>
@@ -4858,7 +4930,7 @@
         <v>96</v>
       </c>
       <c r="K45" s="4" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="L45" s="4" t="s">
         <v>31</v>
@@ -4885,27 +4957,27 @@
         <v>32</v>
       </c>
       <c r="T45" s="4" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="U45" s="4" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="46" spans="1:21" ht="14.45">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A46" s="4" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="C46" s="24" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="D46" s="12" t="s">
         <v>24</v>
       </c>
       <c r="E46" s="12" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="F46" s="4" t="s">
         <v>154</v>
@@ -4920,10 +4992,10 @@
         <v>53</v>
       </c>
       <c r="J46" s="4" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="K46" s="4" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="L46" s="4" t="s">
         <v>33</v>
@@ -4950,27 +5022,27 @@
         <v>28</v>
       </c>
       <c r="T46" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="U46" s="2" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="47" spans="1:21" ht="14.45">
+    <row r="47" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A47" s="4" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="B47" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="C47" s="24" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="D47" s="12" t="s">
         <v>24</v>
       </c>
       <c r="E47" s="12" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="F47" s="4" t="s">
         <v>86</v>
@@ -4985,10 +5057,10 @@
         <v>53</v>
       </c>
       <c r="J47" s="4" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="K47" s="4" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="L47" s="4" t="s">
         <v>31</v>
@@ -5015,27 +5087,27 @@
         <v>28</v>
       </c>
       <c r="T47" t="s">
+        <v>350</v>
+      </c>
+      <c r="U47" s="4" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A48" s="4" t="s">
+        <v>352</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="C48" s="24" t="s">
         <v>354</v>
-      </c>
-      <c r="U47" s="4" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="48" spans="1:21" ht="15.75">
-      <c r="A48" s="4" t="s">
-        <v>356</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>357</v>
-      </c>
-      <c r="C48" s="24" t="s">
-        <v>358</v>
       </c>
       <c r="D48" s="12" t="s">
         <v>24</v>
       </c>
       <c r="E48" s="12" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="F48" s="4" t="s">
         <v>154</v>
@@ -5050,10 +5122,10 @@
         <v>53</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="K48" s="4" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="L48" s="4" t="s">
         <v>33</v>
@@ -5080,27 +5152,27 @@
         <v>28</v>
       </c>
       <c r="T48" t="s">
+        <v>358</v>
+      </c>
+      <c r="U48" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A49" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>361</v>
+      </c>
+      <c r="C49" s="24" t="s">
         <v>362</v>
-      </c>
-      <c r="U48" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="49" spans="1:21" ht="14.45">
-      <c r="A49" s="4" t="s">
-        <v>364</v>
-      </c>
-      <c r="B49" s="8" t="s">
-        <v>365</v>
-      </c>
-      <c r="C49" s="24" t="s">
-        <v>366</v>
       </c>
       <c r="D49" s="12" t="s">
         <v>24</v>
       </c>
       <c r="E49" s="12" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="F49" s="4" t="s">
         <v>154</v>
@@ -5115,10 +5187,10 @@
         <v>53</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="K49" s="4" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="L49" s="4" t="s">
         <v>33</v>
@@ -5145,27 +5217,27 @@
         <v>28</v>
       </c>
       <c r="T49" t="s">
+        <v>365</v>
+      </c>
+      <c r="U49" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A50" s="4" t="s">
+        <v>367</v>
+      </c>
+      <c r="B50" t="s">
+        <v>368</v>
+      </c>
+      <c r="C50" s="24" t="s">
         <v>369</v>
-      </c>
-      <c r="U49" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="50" spans="1:21" ht="14.45">
-      <c r="A50" s="4" t="s">
-        <v>371</v>
-      </c>
-      <c r="B50" t="s">
-        <v>372</v>
-      </c>
-      <c r="C50" s="24" t="s">
-        <v>373</v>
       </c>
       <c r="D50" s="12" t="s">
         <v>24</v>
       </c>
       <c r="E50" s="12" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="F50" s="4" t="s">
         <v>70</v>
@@ -5180,7 +5252,7 @@
         <v>53</v>
       </c>
       <c r="J50" s="4" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="K50" s="4" t="s">
         <v>89</v>
@@ -5210,27 +5282,27 @@
         <v>32</v>
       </c>
       <c r="T50" t="s">
+        <v>371</v>
+      </c>
+      <c r="U50" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A51" s="4" t="s">
+        <v>373</v>
+      </c>
+      <c r="B51" t="s">
+        <v>374</v>
+      </c>
+      <c r="C51" s="24" t="s">
         <v>375</v>
-      </c>
-      <c r="U50" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="51" spans="1:21" ht="14.45">
-      <c r="A51" s="4" t="s">
-        <v>377</v>
-      </c>
-      <c r="B51" t="s">
-        <v>378</v>
-      </c>
-      <c r="C51" s="24" t="s">
-        <v>379</v>
       </c>
       <c r="D51" s="12" t="s">
         <v>24</v>
       </c>
       <c r="E51" s="12" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="F51" s="4" t="s">
         <v>26</v>
@@ -5248,7 +5320,7 @@
         <v>88</v>
       </c>
       <c r="K51" s="4" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="L51" s="4" t="s">
         <v>31</v>
@@ -5275,27 +5347,27 @@
         <v>32</v>
       </c>
       <c r="T51" t="s">
+        <v>378</v>
+      </c>
+      <c r="U51" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A52" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="B52" t="s">
+        <v>381</v>
+      </c>
+      <c r="C52" s="24" t="s">
         <v>382</v>
-      </c>
-      <c r="U51" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="52" spans="1:21" ht="14.45">
-      <c r="A52" s="4" t="s">
-        <v>384</v>
-      </c>
-      <c r="B52" t="s">
-        <v>385</v>
-      </c>
-      <c r="C52" s="24" t="s">
-        <v>386</v>
       </c>
       <c r="D52" s="12" t="s">
         <v>24</v>
       </c>
       <c r="E52" s="12" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="F52" s="4" t="s">
         <v>41</v>
@@ -5340,30 +5412,30 @@
         <v>32</v>
       </c>
       <c r="T52" t="s">
+        <v>384</v>
+      </c>
+      <c r="U52" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A53" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="C53" s="24" t="s">
         <v>388</v>
-      </c>
-      <c r="U52" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="53" spans="1:21" ht="14.45">
-      <c r="A53" s="4" t="s">
-        <v>390</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="C53" s="24" t="s">
-        <v>392</v>
       </c>
       <c r="D53" s="12" t="s">
         <v>24</v>
       </c>
       <c r="E53" s="12" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="G53" s="4" t="s">
         <v>42</v>
@@ -5375,10 +5447,10 @@
         <v>53</v>
       </c>
       <c r="J53" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="K53" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="L53" s="4" t="s">
         <v>31</v>
@@ -5405,30 +5477,30 @@
         <v>32</v>
       </c>
       <c r="T53" t="s">
+        <v>392</v>
+      </c>
+      <c r="U53" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="54" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A54" s="4" t="s">
+        <v>394</v>
+      </c>
+      <c r="B54" t="s">
+        <v>395</v>
+      </c>
+      <c r="C54" s="24" t="s">
         <v>396</v>
-      </c>
-      <c r="U53" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="54" spans="1:21" ht="14.45">
-      <c r="A54" s="4" t="s">
-        <v>398</v>
-      </c>
-      <c r="B54" t="s">
-        <v>399</v>
-      </c>
-      <c r="C54" s="24" t="s">
-        <v>400</v>
       </c>
       <c r="D54" s="12" t="s">
         <v>24</v>
       </c>
       <c r="E54" s="12" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="G54" s="4" t="s">
         <v>42</v>
@@ -5443,7 +5515,7 @@
         <v>96</v>
       </c>
       <c r="K54" s="4" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="L54" s="4" t="s">
         <v>31</v>
@@ -5470,30 +5542,30 @@
         <v>28</v>
       </c>
       <c r="T54" t="s">
+        <v>399</v>
+      </c>
+      <c r="U54" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="55" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A55" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>402</v>
+      </c>
+      <c r="C55" s="24" t="s">
         <v>403</v>
-      </c>
-      <c r="U54" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="55" spans="1:21" ht="14.45">
-      <c r="A55" s="4" t="s">
-        <v>405</v>
-      </c>
-      <c r="B55" s="4" t="s">
-        <v>406</v>
-      </c>
-      <c r="C55" s="24" t="s">
-        <v>407</v>
       </c>
       <c r="D55" s="12" t="s">
         <v>24</v>
       </c>
       <c r="E55" s="12" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="G55" s="4" t="s">
         <v>42</v>
@@ -5508,7 +5580,7 @@
         <v>89</v>
       </c>
       <c r="K55" s="4" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="L55" s="4" t="s">
         <v>31</v>
@@ -5535,27 +5607,27 @@
         <v>28</v>
       </c>
       <c r="T55" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="U55" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="56" spans="1:21" ht="14.45">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="56" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A56" s="4" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="C56" s="24" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="D56" s="12" t="s">
         <v>24</v>
       </c>
       <c r="E56" s="12" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="F56" s="4" t="s">
         <v>154</v>
@@ -5570,10 +5642,10 @@
         <v>53</v>
       </c>
       <c r="J56" s="4" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="K56" s="4" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="L56" s="4" t="s">
         <v>33</v>
@@ -5600,30 +5672,30 @@
         <v>28</v>
       </c>
       <c r="T56" t="s">
+        <v>412</v>
+      </c>
+      <c r="U56" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="57" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A57" s="4" t="s">
+        <v>414</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>415</v>
+      </c>
+      <c r="C57" s="24" t="s">
         <v>416</v>
-      </c>
-      <c r="U56" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="57" spans="1:21" ht="14.45">
-      <c r="A57" s="4" t="s">
-        <v>418</v>
-      </c>
-      <c r="B57" s="4" t="s">
-        <v>419</v>
-      </c>
-      <c r="C57" s="24" t="s">
-        <v>420</v>
       </c>
       <c r="D57" s="14" t="s">
         <v>24</v>
       </c>
       <c r="E57" s="14" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="G57" s="4" t="s">
         <v>42</v>
@@ -5635,7 +5707,7 @@
         <v>53</v>
       </c>
       <c r="J57" s="4" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="K57" s="4" t="s">
         <v>89</v>
@@ -5665,141 +5737,327 @@
         <v>32</v>
       </c>
       <c r="T57" s="4" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="U57" s="4" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="58" spans="1:21" ht="14.45"/>
-    <row r="59" spans="1:21" ht="14.45"/>
-    <row r="60" spans="1:21" ht="14.45"/>
-    <row r="61" spans="1:21" ht="14.45"/>
-    <row r="62" spans="1:21" ht="14.45"/>
-    <row r="63" spans="1:21" ht="14.45"/>
-    <row r="64" spans="1:21" ht="14.45"/>
-    <row r="65" ht="14.45"/>
-    <row r="66" ht="14.45"/>
-    <row r="67" ht="14.45"/>
-    <row r="68" ht="14.45"/>
-    <row r="69" ht="14.45"/>
-    <row r="70" ht="14.45"/>
-    <row r="71" ht="14.45"/>
-    <row r="72" ht="14.45"/>
-    <row r="73" ht="14.45"/>
-    <row r="74" ht="14.45"/>
-    <row r="75" ht="14.45"/>
-    <row r="76" ht="14.45"/>
-    <row r="77" ht="14.45"/>
-    <row r="78" ht="14.45"/>
-    <row r="79" ht="14.45"/>
-    <row r="80" ht="14.45"/>
-    <row r="81" ht="14.45"/>
-    <row r="82" ht="14.45"/>
-    <row r="83" ht="14.45"/>
-    <row r="84" ht="14.45"/>
-    <row r="85" ht="14.45"/>
-    <row r="86" ht="14.45"/>
-    <row r="87" ht="14.45"/>
-    <row r="88" ht="14.45"/>
-    <row r="89" ht="14.45"/>
-    <row r="90" ht="14.45"/>
-    <row r="91" ht="14.45"/>
-    <row r="92" ht="14.45"/>
-    <row r="93" ht="14.45"/>
-    <row r="94" ht="14.45"/>
-    <row r="95" ht="14.45"/>
-    <row r="96" ht="14.45"/>
-    <row r="97" ht="14.45"/>
-    <row r="98" ht="14.45"/>
-    <row r="99" ht="14.45"/>
-    <row r="100" ht="14.45"/>
-    <row r="101" ht="14.45"/>
-    <row r="102" ht="14.45"/>
-    <row r="103" ht="14.45"/>
-    <row r="104" ht="14.45"/>
-    <row r="105" ht="14.45"/>
-    <row r="106" ht="14.45"/>
-    <row r="107" ht="14.45"/>
-    <row r="108" ht="14.45"/>
-    <row r="109" ht="14.45"/>
-    <row r="110" ht="14.45"/>
-    <row r="111" ht="14.45"/>
-    <row r="112" ht="14.45"/>
-    <row r="113" ht="14.45"/>
-    <row r="114" ht="14.45"/>
-    <row r="115" ht="14.45"/>
-    <row r="116" ht="14.45"/>
-    <row r="117" ht="14.45"/>
-    <row r="118" ht="14.45"/>
-    <row r="119" ht="14.45"/>
-    <row r="120" ht="14.45"/>
-    <row r="121" ht="14.45"/>
-    <row r="122" ht="14.45"/>
-    <row r="123" ht="14.45"/>
-    <row r="124" ht="14.45"/>
-    <row r="125" ht="14.45"/>
-    <row r="126" ht="14.45"/>
-    <row r="127" ht="14.45"/>
-    <row r="128" ht="14.45"/>
-    <row r="129" ht="14.45"/>
-    <row r="130" ht="14.45"/>
-    <row r="131" ht="14.45"/>
-    <row r="132" ht="14.45"/>
-    <row r="133" ht="14.45"/>
-    <row r="134" ht="14.45"/>
-    <row r="135" ht="14.45"/>
-    <row r="136" ht="14.45"/>
-    <row r="137" ht="14.45"/>
-    <row r="138" ht="14.45"/>
-    <row r="139" ht="14.45"/>
-    <row r="140" ht="14.45"/>
-    <row r="141" ht="14.45"/>
-    <row r="142" ht="14.45"/>
-    <row r="143" ht="14.45"/>
-    <row r="144" ht="14.45"/>
-    <row r="145" ht="14.45"/>
-    <row r="146" ht="14.45"/>
-    <row r="147" ht="14.45"/>
-    <row r="148" ht="14.45"/>
-    <row r="149" ht="14.45"/>
-    <row r="150" ht="14.45"/>
-    <row r="151" ht="14.45"/>
-    <row r="152" ht="14.45"/>
-    <row r="153" ht="14.45"/>
-    <row r="154" ht="14.45"/>
-    <row r="155" ht="14.45"/>
-    <row r="156" ht="14.45"/>
-    <row r="157" ht="14.45"/>
-    <row r="158" ht="14.45"/>
-    <row r="159" ht="14.45"/>
-    <row r="160" ht="14.45"/>
-    <row r="161" ht="14.45"/>
-    <row r="162" ht="14.45"/>
-    <row r="163" ht="14.45"/>
-    <row r="164" ht="14.45"/>
-    <row r="165" ht="14.45"/>
-    <row r="166" ht="14.45"/>
-    <row r="167" ht="14.45"/>
-    <row r="168" ht="14.45"/>
-    <row r="169" ht="14.45"/>
-    <row r="170" ht="14.45"/>
-    <row r="171" ht="14.45"/>
-    <row r="172" ht="14.45"/>
-    <row r="173" ht="14.45"/>
-    <row r="174" ht="14.45"/>
-    <row r="175" ht="14.45"/>
-    <row r="176" ht="14.45"/>
-    <row r="177" ht="14.45"/>
-    <row r="178" ht="14.45"/>
-    <row r="179" ht="14.45"/>
-    <row r="180" ht="14.45"/>
-    <row r="181" ht="14.45"/>
-    <row r="182" ht="14.45"/>
-    <row r="183" ht="14.45"/>
-    <row r="184" ht="14.45"/>
-    <row r="185" ht="14.45"/>
-    <row r="186" ht="14.45"/>
+        <v>420</v>
+      </c>
+    </row>
+    <row r="58" spans="1:21" s="26" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A58" s="25" t="s">
+        <v>470</v>
+      </c>
+      <c r="B58" s="25" t="s">
+        <v>472</v>
+      </c>
+      <c r="C58" s="25" t="s">
+        <v>485</v>
+      </c>
+      <c r="D58" s="25"/>
+      <c r="E58" s="27" t="s">
+        <v>488</v>
+      </c>
+      <c r="F58" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="G58" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="H58" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="I58" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="J58" s="25" t="s">
+        <v>473</v>
+      </c>
+      <c r="K58" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="L58" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="M58" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="N58" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="O58" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="P58" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q58" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="R58" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="S58" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="T58" s="25" t="s">
+        <v>474</v>
+      </c>
+      <c r="U58" s="25" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="59" spans="1:21" s="26" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A59" s="25" t="s">
+        <v>471</v>
+      </c>
+      <c r="B59" s="25" t="s">
+        <v>476</v>
+      </c>
+      <c r="C59" s="25" t="s">
+        <v>486</v>
+      </c>
+      <c r="D59" s="25"/>
+      <c r="E59" s="27" t="s">
+        <v>490</v>
+      </c>
+      <c r="F59" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="G59" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="H59" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="I59" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="J59" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="K59" s="25" t="s">
+        <v>477</v>
+      </c>
+      <c r="L59" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="M59" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="N59" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="O59" s="25" t="s">
+        <v>189</v>
+      </c>
+      <c r="P59" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q59" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="R59" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="S59" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="T59" s="25" t="s">
+        <v>478</v>
+      </c>
+      <c r="U59" s="25" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="60" spans="1:21" s="26" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A60" s="25" t="s">
+        <v>480</v>
+      </c>
+      <c r="B60" s="25" t="s">
+        <v>481</v>
+      </c>
+      <c r="C60" s="25" t="s">
+        <v>487</v>
+      </c>
+      <c r="D60" s="25"/>
+      <c r="E60" s="27" t="s">
+        <v>489</v>
+      </c>
+      <c r="F60" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="G60" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="H60" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="I60" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="J60" s="25" t="s">
+        <v>482</v>
+      </c>
+      <c r="K60" s="25" t="s">
+        <v>483</v>
+      </c>
+      <c r="L60" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="M60" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="N60" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="O60" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="P60" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q60" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="R60" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="S60" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="T60" s="25" t="s">
+        <v>475</v>
+      </c>
+      <c r="U60" s="25" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="61" spans="1:21" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="62" spans="1:21" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="63" spans="1:21" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="64" spans="1:21" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="65" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="66" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="67" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="68" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="69" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="70" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="71" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="72" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="73" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="74" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="75" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="76" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="77" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="78" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="79" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="80" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="81" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="82" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="83" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="84" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="85" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="86" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="87" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="88" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="89" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="90" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="91" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="92" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="93" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="94" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="95" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="96" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="97" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="98" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="99" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="100" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="101" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="102" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="103" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="104" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="105" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="106" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="107" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="108" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="109" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="110" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="111" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="112" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="113" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="114" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="115" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="116" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="117" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="118" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="119" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="120" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="121" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="122" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="123" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="124" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="125" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="126" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="127" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="128" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="129" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="130" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="131" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="132" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="133" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="134" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="135" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="136" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="137" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="138" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="139" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="140" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="141" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="142" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="143" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="144" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="145" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="146" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="147" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="148" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="149" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="150" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="151" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="152" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="153" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="154" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="155" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="156" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="157" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="158" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="159" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="160" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="161" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="162" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="163" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="164" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="165" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="166" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="167" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="168" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="169" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="170" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="171" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="172" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="173" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="174" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="175" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="176" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="177" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="178" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="179" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="180" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="181" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="182" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="183" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="184" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="185" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="186" ht="14.5" x14ac:dyDescent="0.35"/>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:U45">
     <sortCondition ref="A2:A45"/>
@@ -5946,6 +6204,9 @@
     <hyperlink ref="E37" r:id="rId111" xr:uid="{B9227BF6-565E-4CC0-BF4C-4C508A7DB46B}"/>
     <hyperlink ref="D57" r:id="rId112" xr:uid="{B6DDFCF8-2D59-4DA8-9C7A-A1B7B7E26168}"/>
     <hyperlink ref="E57" r:id="rId113" xr:uid="{42C95BBC-98B4-4E80-B097-88E6F392B903}"/>
+    <hyperlink ref="E58" r:id="rId114" xr:uid="{4F00AB62-1372-499A-8211-9711806AABEA}"/>
+    <hyperlink ref="E59" r:id="rId115" xr:uid="{F708A31D-C2B5-4330-AF9A-C16DA58EC2AE}"/>
+    <hyperlink ref="E60" r:id="rId116" xr:uid="{14D81D35-D16E-4182-94FC-43E955C1B5D3}"/>
   </hyperlinks>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5964,761 +6225,761 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" customWidth="1"/>
-    <col min="2" max="2" width="50.42578125" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" customWidth="1"/>
-    <col min="5" max="5" width="34.28515625" style="11" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.54296875" customWidth="1"/>
+    <col min="2" max="2" width="50.453125" customWidth="1"/>
+    <col min="3" max="3" width="18.1796875" customWidth="1"/>
+    <col min="4" max="4" width="16.7265625" customWidth="1"/>
+    <col min="5" max="5" width="34.26953125" style="11" customWidth="1"/>
+    <col min="6" max="6" width="9.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="20" customFormat="1" ht="26.25" customHeight="1">
+    <row r="1" spans="1:5" s="20" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="20" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="20" customFormat="1" ht="50.25" customHeight="1">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="20" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="D2" s="21"/>
       <c r="E2" s="21"/>
     </row>
-    <row r="3" spans="1:5" s="20" customFormat="1" ht="50.25" customHeight="1">
+    <row r="3" spans="1:5" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="20" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="21"/>
     </row>
-    <row r="4" spans="1:5" s="20" customFormat="1" ht="50.25" customHeight="1">
+    <row r="4" spans="1:5" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="D4" s="22"/>
       <c r="E4" s="21"/>
     </row>
-    <row r="5" spans="1:5" s="20" customFormat="1" ht="50.25" customHeight="1">
+    <row r="5" spans="1:5" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="B5" s="21"/>
       <c r="D5" s="21"/>
       <c r="E5" s="21"/>
     </row>
-    <row r="6" spans="1:5" s="20" customFormat="1" ht="50.25" customHeight="1">
+    <row r="6" spans="1:5" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="20" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="D6" s="21"/>
       <c r="E6" s="21"/>
     </row>
-    <row r="7" spans="1:5" s="20" customFormat="1" ht="50.25" customHeight="1">
+    <row r="7" spans="1:5" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="20" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="D7" s="22"/>
       <c r="E7" s="21"/>
     </row>
-    <row r="8" spans="1:5" s="20" customFormat="1" ht="50.25" customHeight="1">
+    <row r="8" spans="1:5" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="20" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="D8" s="22"/>
       <c r="E8" s="21"/>
     </row>
-    <row r="9" spans="1:5" s="20" customFormat="1" ht="50.25" customHeight="1">
+    <row r="9" spans="1:5" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="20" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="D9" s="21"/>
       <c r="E9" s="21"/>
     </row>
-    <row r="10" spans="1:5" s="20" customFormat="1" ht="50.25" customHeight="1">
+    <row r="10" spans="1:5" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="20" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="B10" s="21"/>
       <c r="D10" s="21"/>
       <c r="E10" s="21"/>
     </row>
-    <row r="11" spans="1:5" s="20" customFormat="1" ht="50.25" customHeight="1">
+    <row r="11" spans="1:5" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="20" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="D11" s="22"/>
       <c r="E11" s="21"/>
     </row>
-    <row r="12" spans="1:5" s="20" customFormat="1" ht="50.25" customHeight="1">
+    <row r="12" spans="1:5" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="20" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="B12" s="23"/>
       <c r="D12" s="22"/>
       <c r="E12" s="21"/>
     </row>
-    <row r="13" spans="1:5" s="20" customFormat="1" ht="50.25" customHeight="1">
+    <row r="13" spans="1:5" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="20" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="D13" s="21"/>
       <c r="E13" s="21"/>
     </row>
-    <row r="14" spans="1:5" s="20" customFormat="1" ht="50.25" customHeight="1">
+    <row r="14" spans="1:5" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="20" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="D14" s="22"/>
       <c r="E14" s="21"/>
     </row>
-    <row r="15" spans="1:5" s="20" customFormat="1" ht="50.25" customHeight="1">
+    <row r="15" spans="1:5" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="20" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="D15" s="22"/>
       <c r="E15" s="21"/>
     </row>
-    <row r="16" spans="1:5" s="20" customFormat="1" ht="50.25" customHeight="1">
+    <row r="16" spans="1:5" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="20" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="D16" s="21"/>
       <c r="E16" s="21"/>
     </row>
-    <row r="17" spans="1:5" s="20" customFormat="1" ht="50.25" customHeight="1">
+    <row r="17" spans="1:5" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="20" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="B17" s="21"/>
       <c r="D17" s="21"/>
       <c r="E17" s="21"/>
     </row>
-    <row r="18" spans="1:5" s="20" customFormat="1" ht="50.25" customHeight="1">
+    <row r="18" spans="1:5" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="20" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="D18" s="21"/>
       <c r="E18" s="21"/>
     </row>
-    <row r="19" spans="1:5" s="20" customFormat="1" ht="50.25" customHeight="1">
+    <row r="19" spans="1:5" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="20" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="D19" s="21"/>
       <c r="E19" s="21"/>
     </row>
-    <row r="20" spans="1:5" s="20" customFormat="1" ht="50.25" customHeight="1">
+    <row r="20" spans="1:5" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="20" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="D20" s="21"/>
       <c r="E20" s="21"/>
     </row>
-    <row r="21" spans="1:5" s="20" customFormat="1" ht="50.25" customHeight="1">
+    <row r="21" spans="1:5" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="20" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="D21" s="21"/>
       <c r="E21" s="21"/>
     </row>
-    <row r="22" spans="1:5" s="20" customFormat="1" ht="50.25" customHeight="1">
+    <row r="22" spans="1:5" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="20" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="D22" s="21"/>
       <c r="E22" s="21"/>
     </row>
-    <row r="23" spans="1:5" s="20" customFormat="1" ht="50.25" customHeight="1">
+    <row r="23" spans="1:5" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="20" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="D23" s="21"/>
       <c r="E23" s="21"/>
     </row>
-    <row r="24" spans="1:5" s="20" customFormat="1" ht="50.25" customHeight="1">
+    <row r="24" spans="1:5" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="20" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="D24" s="21"/>
       <c r="E24" s="21"/>
     </row>
-    <row r="25" spans="1:5" s="20" customFormat="1" ht="50.25" customHeight="1">
+    <row r="25" spans="1:5" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="20" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="D25" s="21"/>
       <c r="E25" s="21"/>
     </row>
-    <row r="26" spans="1:5" s="20" customFormat="1" ht="50.25" customHeight="1">
+    <row r="26" spans="1:5" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="20" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="D26" s="21"/>
       <c r="E26" s="21"/>
     </row>
-    <row r="27" spans="1:5" s="20" customFormat="1" ht="50.25" customHeight="1">
+    <row r="27" spans="1:5" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="20" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="D27" s="21"/>
       <c r="E27" s="21"/>
     </row>
-    <row r="28" spans="1:5" s="20" customFormat="1" ht="50.25" customHeight="1">
+    <row r="28" spans="1:5" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="20" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="D28" s="21"/>
       <c r="E28" s="21"/>
     </row>
-    <row r="29" spans="1:5" s="20" customFormat="1" ht="50.25" customHeight="1">
+    <row r="29" spans="1:5" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="20" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="D29" s="21"/>
       <c r="E29" s="21"/>
     </row>
-    <row r="30" spans="1:5" s="20" customFormat="1" ht="50.25" customHeight="1">
+    <row r="30" spans="1:5" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="20" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="D30" s="21"/>
       <c r="E30" s="21"/>
     </row>
-    <row r="31" spans="1:5" s="20" customFormat="1" ht="50.25" customHeight="1">
+    <row r="31" spans="1:5" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="20" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="D31" s="21"/>
       <c r="E31" s="21"/>
     </row>
-    <row r="32" spans="1:5" s="20" customFormat="1" ht="50.25" customHeight="1">
+    <row r="32" spans="1:5" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="20" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="D32" s="21"/>
       <c r="E32" s="21"/>
     </row>
-    <row r="33" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1">
+    <row r="33" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="20" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="B33" s="21"/>
       <c r="D33" s="21"/>
       <c r="E33" s="21"/>
     </row>
-    <row r="34" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1">
+    <row r="34" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="20" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="D34" s="21"/>
       <c r="E34" s="21"/>
     </row>
-    <row r="35" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1">
+    <row r="35" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="20" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="D35" s="21"/>
       <c r="E35" s="21"/>
     </row>
-    <row r="36" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1">
+    <row r="36" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="20" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="D36" s="21"/>
       <c r="E36" s="21"/>
     </row>
-    <row r="37" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1">
+    <row r="37" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="20" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="D37" s="21"/>
       <c r="E37" s="21"/>
     </row>
-    <row r="38" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1">
+    <row r="38" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="20" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="D38" s="21"/>
       <c r="E38" s="21"/>
     </row>
-    <row r="39" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1">
+    <row r="39" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="20" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="D39" s="21"/>
       <c r="E39" s="21"/>
     </row>
-    <row r="40" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1">
+    <row r="40" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="20" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="D40" s="21"/>
       <c r="E40" s="21"/>
     </row>
-    <row r="41" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1">
+    <row r="41" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="20" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="D41" s="21"/>
       <c r="E41" s="21"/>
     </row>
-    <row r="42" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1">
+    <row r="42" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="20" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="D42" s="21"/>
       <c r="E42" s="21"/>
     </row>
-    <row r="43" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1">
+    <row r="43" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="20" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="D43" s="21"/>
       <c r="E43" s="21"/>
     </row>
-    <row r="44" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1">
+    <row r="44" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="20" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="D44" s="21"/>
       <c r="E44" s="21"/>
     </row>
-    <row r="45" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1">
+    <row r="45" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="20" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="D45" s="21"/>
       <c r="E45" s="21"/>
     </row>
-    <row r="46" spans="1:6" ht="14.45">
+    <row r="46" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="D46" s="16"/>
       <c r="E46" s="17"/>
       <c r="F46" s="1"/>
     </row>
-    <row r="47" spans="1:6" ht="14.45">
+    <row r="47" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="D47" s="16"/>
       <c r="E47" s="17"/>
       <c r="F47" s="1"/>
     </row>
-    <row r="48" spans="1:6" ht="14.45">
+    <row r="48" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E48" s="18"/>
       <c r="F48" s="1"/>
     </row>
-    <row r="49" spans="5:6" ht="14.45">
+    <row r="49" spans="5:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E49" s="18"/>
       <c r="F49" s="1"/>
     </row>
-    <row r="50" spans="5:6" ht="14.45">
+    <row r="50" spans="5:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E50" s="18"/>
       <c r="F50" s="1"/>
     </row>
-    <row r="51" spans="5:6" ht="14.45">
+    <row r="51" spans="5:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E51" s="18"/>
       <c r="F51" s="1"/>
     </row>
-    <row r="52" spans="5:6" ht="14.45">
+    <row r="52" spans="5:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E52" s="18"/>
       <c r="F52" s="1"/>
     </row>
-    <row r="53" spans="5:6" ht="14.45">
+    <row r="53" spans="5:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E53" s="18"/>
       <c r="F53" s="1"/>
     </row>
-    <row r="54" spans="5:6" ht="14.45">
+    <row r="54" spans="5:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E54" s="18"/>
       <c r="F54" s="1"/>
     </row>
-    <row r="55" spans="5:6" ht="14.45">
+    <row r="55" spans="5:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E55" s="18"/>
       <c r="F55" s="1"/>
     </row>
-    <row r="56" spans="5:6" ht="14.45">
+    <row r="56" spans="5:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E56" s="18"/>
       <c r="F56" s="1"/>
     </row>
-    <row r="57" spans="5:6" ht="14.45">
+    <row r="57" spans="5:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E57" s="18"/>
       <c r="F57" s="1"/>
     </row>
-    <row r="58" spans="5:6" ht="14.45">
+    <row r="58" spans="5:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E58" s="18"/>
       <c r="F58" s="1"/>
     </row>
-    <row r="59" spans="5:6" ht="14.45">
+    <row r="59" spans="5:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E59" s="18"/>
       <c r="F59" s="1"/>
     </row>
-    <row r="60" spans="5:6" ht="14.45">
+    <row r="60" spans="5:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E60" s="18"/>
       <c r="F60" s="1"/>
     </row>
-    <row r="61" spans="5:6" ht="14.45">
+    <row r="61" spans="5:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E61" s="18"/>
       <c r="F61" s="1"/>
     </row>
-    <row r="62" spans="5:6" ht="14.45">
+    <row r="62" spans="5:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E62" s="18"/>
       <c r="F62" s="1"/>
     </row>
-    <row r="63" spans="5:6" ht="14.45">
+    <row r="63" spans="5:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E63" s="18"/>
       <c r="F63" s="1"/>
     </row>
-    <row r="64" spans="5:6" ht="14.45">
+    <row r="64" spans="5:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E64" s="18"/>
       <c r="F64" s="1"/>
     </row>
-    <row r="65" spans="5:6" ht="14.45">
+    <row r="65" spans="5:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E65" s="18"/>
       <c r="F65" s="1"/>
     </row>
-    <row r="66" spans="5:6" ht="14.45">
+    <row r="66" spans="5:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E66" s="18"/>
       <c r="F66" s="1"/>
     </row>
-    <row r="67" spans="5:6" ht="14.45">
+    <row r="67" spans="5:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E67" s="18"/>
       <c r="F67" s="1"/>
     </row>
-    <row r="68" spans="5:6" ht="14.45">
+    <row r="68" spans="5:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E68" s="18"/>
       <c r="F68" s="1"/>
     </row>
-    <row r="69" spans="5:6" ht="14.45">
+    <row r="69" spans="5:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E69" s="18"/>
       <c r="F69" s="1"/>
     </row>
-    <row r="70" spans="5:6" ht="14.45">
+    <row r="70" spans="5:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E70" s="18"/>
       <c r="F70" s="1"/>
     </row>
-    <row r="71" spans="5:6" ht="14.45">
+    <row r="71" spans="5:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E71" s="18"/>
       <c r="F71" s="1"/>
     </row>
-    <row r="72" spans="5:6" ht="14.45">
+    <row r="72" spans="5:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E72" s="18"/>
       <c r="F72" s="1"/>
     </row>
-    <row r="73" spans="5:6" ht="14.45">
+    <row r="73" spans="5:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E73" s="18"/>
       <c r="F73" s="1"/>
     </row>
-    <row r="74" spans="5:6" ht="14.45">
+    <row r="74" spans="5:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="F74" s="1"/>
     </row>
-    <row r="75" spans="5:6" ht="14.45">
+    <row r="75" spans="5:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="F75" s="1"/>
     </row>
-    <row r="76" spans="5:6" ht="14.45">
+    <row r="76" spans="5:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="F76" s="1"/>
     </row>
-    <row r="77" spans="5:6" ht="14.45">
+    <row r="77" spans="5:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="F77" s="1"/>
     </row>
-    <row r="78" spans="5:6" ht="14.45">
+    <row r="78" spans="5:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="F78" s="1"/>
     </row>
-    <row r="79" spans="5:6" ht="14.45">
+    <row r="79" spans="5:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="F79" s="1"/>
     </row>
-    <row r="80" spans="5:6" ht="14.45">
+    <row r="80" spans="5:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="F80" s="1"/>
     </row>
-    <row r="81" spans="5:6" ht="14.45">
+    <row r="81" spans="5:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="F81" s="1"/>
     </row>
-    <row r="82" spans="5:6" ht="14.45">
+    <row r="82" spans="5:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="F82" s="1"/>
     </row>
-    <row r="83" spans="5:6" ht="14.45">
+    <row r="83" spans="5:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="F83" s="1"/>
     </row>
-    <row r="84" spans="5:6" ht="14.45">
+    <row r="84" spans="5:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="F84" s="1"/>
     </row>
-    <row r="85" spans="5:6" ht="14.45">
+    <row r="85" spans="5:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="F85" s="1"/>
     </row>
-    <row r="86" spans="5:6" ht="14.45">
+    <row r="86" spans="5:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="F86" s="1"/>
     </row>
-    <row r="87" spans="5:6" ht="14.45">
+    <row r="87" spans="5:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="F87" s="1"/>
     </row>
-    <row r="88" spans="5:6" ht="14.45">
+    <row r="88" spans="5:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="F88" s="1"/>
     </row>
-    <row r="89" spans="5:6" ht="14.45">
+    <row r="89" spans="5:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="F89" s="1"/>
     </row>
-    <row r="90" spans="5:6" ht="14.45">
+    <row r="90" spans="5:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="F90" s="1"/>
     </row>
-    <row r="91" spans="5:6" ht="14.45">
+    <row r="91" spans="5:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="F91" s="1"/>
     </row>
-    <row r="92" spans="5:6" ht="14.45">
+    <row r="92" spans="5:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="F92" s="1"/>
     </row>
-    <row r="93" spans="5:6" ht="14.45">
+    <row r="93" spans="5:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="F93" s="1"/>
     </row>
-    <row r="94" spans="5:6" ht="15.6">
+    <row r="94" spans="5:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="E94" s="19"/>
       <c r="F94" s="1"/>
     </row>
-    <row r="95" spans="5:6" ht="15.6">
+    <row r="95" spans="5:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="E95" s="19"/>
       <c r="F95" s="1"/>
     </row>
-    <row r="96" spans="5:6" ht="15.6">
+    <row r="96" spans="5:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="E96" s="19"/>
       <c r="F96" s="1"/>
     </row>
-    <row r="97" spans="5:6" ht="15.6">
+    <row r="97" spans="5:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="E97" s="19"/>
       <c r="F97" s="1"/>
     </row>
-    <row r="98" spans="5:6" ht="15.6">
+    <row r="98" spans="5:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="E98" s="19"/>
       <c r="F98" s="1"/>
     </row>
-    <row r="99" spans="5:6" ht="15.6">
+    <row r="99" spans="5:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="E99" s="19"/>
       <c r="F99" s="1"/>
     </row>
-    <row r="100" spans="5:6" ht="15.6">
+    <row r="100" spans="5:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="E100" s="19"/>
       <c r="F100" s="1"/>
     </row>
-    <row r="101" spans="5:6" ht="15.6">
+    <row r="101" spans="5:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="E101" s="19"/>
       <c r="F101" s="1"/>
     </row>
-    <row r="102" spans="5:6" ht="15.6">
+    <row r="102" spans="5:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="E102" s="19"/>
       <c r="F102" s="1"/>
     </row>
-    <row r="103" spans="5:6" ht="15.6">
+    <row r="103" spans="5:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="E103" s="19"/>
       <c r="F103" s="1"/>
     </row>
-    <row r="104" spans="5:6" ht="15.6">
+    <row r="104" spans="5:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="E104" s="19"/>
       <c r="F104" s="1"/>
     </row>
-    <row r="105" spans="5:6" ht="15.6">
+    <row r="105" spans="5:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="E105" s="19"/>
       <c r="F105" s="1"/>
     </row>
-    <row r="106" spans="5:6" ht="15.6">
+    <row r="106" spans="5:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="E106" s="19"/>
       <c r="F106" s="1"/>
     </row>
-    <row r="107" spans="5:6" ht="15.6">
+    <row r="107" spans="5:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="E107" s="19"/>
       <c r="F107" s="1"/>
     </row>
-    <row r="108" spans="5:6" ht="15.6">
+    <row r="108" spans="5:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="E108" s="19"/>
       <c r="F108" s="1"/>
     </row>
-    <row r="109" spans="5:6" ht="15.6">
+    <row r="109" spans="5:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="E109" s="19"/>
       <c r="F109" s="1"/>
     </row>
-    <row r="110" spans="5:6" ht="15.6">
+    <row r="110" spans="5:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="E110" s="19"/>
       <c r="F110" s="1"/>
     </row>
-    <row r="111" spans="5:6" ht="15.6">
+    <row r="111" spans="5:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="E111" s="19"/>
       <c r="F111" s="1"/>
     </row>
-    <row r="112" spans="5:6" ht="15.6">
+    <row r="112" spans="5:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="E112" s="19"/>
       <c r="F112" s="1"/>
     </row>
-    <row r="113" spans="5:6" ht="15.6">
+    <row r="113" spans="5:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="E113" s="19"/>
       <c r="F113" s="1"/>
     </row>
-    <row r="114" spans="5:6" ht="14.45">
+    <row r="114" spans="5:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E114" s="18"/>
       <c r="F114" s="1"/>
     </row>
-    <row r="115" spans="5:6" ht="14.45">
+    <row r="115" spans="5:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E115" s="18"/>
       <c r="F115" s="1"/>
     </row>
-    <row r="116" spans="5:6" ht="14.45">
+    <row r="116" spans="5:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E116" s="18"/>
       <c r="F116" s="1"/>
     </row>
-    <row r="117" spans="5:6" ht="14.45">
+    <row r="117" spans="5:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E117" s="18"/>
       <c r="F117" s="1"/>
     </row>
-    <row r="118" spans="5:6" ht="14.45">
+    <row r="118" spans="5:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E118" s="18"/>
       <c r="F118" s="1"/>
     </row>
-    <row r="119" spans="5:6" ht="14.45">
+    <row r="119" spans="5:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E119" s="18"/>
       <c r="F119" s="1"/>
     </row>
-    <row r="120" spans="5:6" ht="14.45">
+    <row r="120" spans="5:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E120" s="18"/>
       <c r="F120" s="1"/>
     </row>
-    <row r="121" spans="5:6" ht="14.45">
+    <row r="121" spans="5:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E121" s="18"/>
       <c r="F121" s="1"/>
     </row>
-    <row r="122" spans="5:6" ht="14.45">
+    <row r="122" spans="5:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E122" s="18"/>
       <c r="F122" s="1"/>
     </row>
-    <row r="123" spans="5:6" ht="14.45">
+    <row r="123" spans="5:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E123" s="18"/>
       <c r="F123" s="1"/>
     </row>
-    <row r="124" spans="5:6" ht="14.45">
+    <row r="124" spans="5:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E124" s="18"/>
       <c r="F124" s="1"/>
     </row>
-    <row r="125" spans="5:6" ht="14.45">
+    <row r="125" spans="5:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E125" s="18"/>
       <c r="F125" s="1"/>
     </row>
-    <row r="126" spans="5:6" ht="14.45">
+    <row r="126" spans="5:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E126" s="18"/>
       <c r="F126" s="1"/>
     </row>
-    <row r="127" spans="5:6" ht="14.45">
+    <row r="127" spans="5:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E127" s="18"/>
       <c r="F127" s="1"/>
     </row>
-    <row r="128" spans="5:6" ht="14.45">
+    <row r="128" spans="5:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E128" s="18"/>
       <c r="F128" s="1"/>
     </row>
-    <row r="129" spans="5:6" ht="14.45">
+    <row r="129" spans="5:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E129" s="18"/>
       <c r="F129" s="1"/>
     </row>
-    <row r="130" spans="5:6" ht="14.45">
+    <row r="130" spans="5:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E130" s="18"/>
       <c r="F130" s="1"/>
     </row>
-    <row r="131" spans="5:6" ht="14.45">
+    <row r="131" spans="5:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E131" s="18"/>
       <c r="F131" s="1"/>
     </row>
-    <row r="132" spans="5:6" ht="14.45">
+    <row r="132" spans="5:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E132" s="18"/>
       <c r="F132" s="1"/>
     </row>
-    <row r="133" spans="5:6" ht="14.45">
+    <row r="133" spans="5:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="F133" s="1"/>
     </row>
-    <row r="134" spans="5:6" ht="14.45">
+    <row r="134" spans="5:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="F134" s="1"/>
     </row>
-    <row r="135" spans="5:6" ht="14.45">
+    <row r="135" spans="5:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="F135" s="1"/>
     </row>
-    <row r="136" spans="5:6" ht="15" customHeight="1">
+    <row r="136" spans="5:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F136" s="1"/>
     </row>
-    <row r="137" spans="5:6" ht="15" customHeight="1">
+    <row r="137" spans="5:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F137" s="1"/>
     </row>
-    <row r="138" spans="5:6" ht="15" customHeight="1">
+    <row r="138" spans="5:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F138" s="1"/>
     </row>
-    <row r="139" spans="5:6" ht="15" customHeight="1">
+    <row r="139" spans="5:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F139" s="1"/>
     </row>
-    <row r="140" spans="5:6" ht="15" customHeight="1">
+    <row r="140" spans="5:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F140" s="1"/>
     </row>
-    <row r="141" spans="5:6" ht="15" customHeight="1">
+    <row r="141" spans="5:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F141" s="1"/>
     </row>
-    <row r="142" spans="5:6" ht="15" customHeight="1">
+    <row r="142" spans="5:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F142" s="1"/>
     </row>
-    <row r="143" spans="5:6" ht="15" customHeight="1">
+    <row r="143" spans="5:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F143" s="1"/>
     </row>
-    <row r="144" spans="5:6" ht="15" customHeight="1">
+    <row r="144" spans="5:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F144" s="1"/>
     </row>
-    <row r="145" spans="6:6" ht="15" customHeight="1">
+    <row r="145" spans="6:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F145" s="1"/>
     </row>
-    <row r="146" spans="6:6" ht="15" customHeight="1">
+    <row r="146" spans="6:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F146" s="1"/>
     </row>
-    <row r="147" spans="6:6" ht="15" customHeight="1">
+    <row r="147" spans="6:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F147" s="1"/>
     </row>
-    <row r="148" spans="6:6" ht="15" customHeight="1">
+    <row r="148" spans="6:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F148" s="1"/>
     </row>
-    <row r="149" spans="6:6" ht="15" customHeight="1">
+    <row r="149" spans="6:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F149" s="1"/>
     </row>
-    <row r="150" spans="6:6" ht="15" customHeight="1">
+    <row r="150" spans="6:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F150" s="1"/>
     </row>
-    <row r="151" spans="6:6" ht="15" customHeight="1">
+    <row r="151" spans="6:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F151" s="1"/>
     </row>
-    <row r="152" spans="6:6" ht="15" customHeight="1">
+    <row r="152" spans="6:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F152" s="1"/>
     </row>
-    <row r="153" spans="6:6" ht="15" customHeight="1">
+    <row r="153" spans="6:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F153" s="1"/>
     </row>
-    <row r="154" spans="6:6" ht="15" customHeight="1">
+    <row r="154" spans="6:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F154" s="1"/>
     </row>
-    <row r="155" spans="6:6" ht="15" customHeight="1">
+    <row r="155" spans="6:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F155" s="1"/>
     </row>
-    <row r="156" spans="6:6" ht="15" customHeight="1">
+    <row r="156" spans="6:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F156" s="1"/>
     </row>
-    <row r="157" spans="6:6" ht="15" customHeight="1">
+    <row r="157" spans="6:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F157" s="1"/>
     </row>
-    <row r="158" spans="6:6" ht="15" customHeight="1">
+    <row r="158" spans="6:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F158" s="1"/>
     </row>
-    <row r="159" spans="6:6" ht="15" customHeight="1">
+    <row r="159" spans="6:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F159" s="1"/>
     </row>
-    <row r="160" spans="6:6" ht="15" customHeight="1">
+    <row r="160" spans="6:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F160" s="1"/>
     </row>
-    <row r="161" spans="6:6" ht="15" customHeight="1">
+    <row r="161" spans="6:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F161" s="1"/>
     </row>
-    <row r="162" spans="6:6" ht="15" customHeight="1">
+    <row r="162" spans="6:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F162" s="1"/>
     </row>
-    <row r="163" spans="6:6" ht="15" customHeight="1">
+    <row r="163" spans="6:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F163" s="1"/>
     </row>
   </sheetData>
@@ -6746,6 +7007,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000D89A625C5B6364BB7302BED22ED65DA" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="05bac8ad6e033965382d52c38353e541">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="7855343b-5261-4afc-a17c-d4c130fbaa85" xmlns:ns4="72f917e0-5d36-43ac-975d-26afa4cf7fc0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="452e5605b09f318b6d66379e79837bd5" ns3:_="" ns4:_="">
     <xsd:import namespace="7855343b-5261-4afc-a17c-d4c130fbaa85"/>
@@ -6992,23 +7262,39 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F53F9CFB-0E7D-4BF1-9CBE-0D133C6536E4}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F53F9CFB-0E7D-4BF1-9CBE-0D133C6536E4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="7855343b-5261-4afc-a17c-d4c130fbaa85"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56978299-3DC6-451D-A1E5-57FB07C431CC}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BE4A15A-EC2D-4537-B6DC-2F235DBE6314}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BE4A15A-EC2D-4537-B6DC-2F235DBE6314}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56978299-3DC6-451D-A1E5-57FB07C431CC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="7855343b-5261-4afc-a17c-d4c130fbaa85"/>
+    <ds:schemaRef ds:uri="72f917e0-5d36-43ac-975d-26afa4cf7fc0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Before & After projects' description added
</commit_message>
<xml_diff>
--- a/data/Outdoor plants.xlsx
+++ b/data/Outdoor plants.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29711"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\landscapingUOB-api\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DCB66FB-5FE2-4ADC-9B70-3E9A3A66800E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B669DAD4-E91F-49F5-A303-CB4B55738398}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{8B519764-563C-4CD5-B8E9-9B8B0702B21B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{8B519764-563C-4CD5-B8E9-9B8B0702B21B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -460,7 +460,7 @@
     <t>نبات المظلة</t>
   </si>
   <si>
-    <t>https://i.postimg.cc/YCtWYXww/Cyperus-aternifolius.jpg</t>
+    <t>https://i.postimg.cc/mrtvb3SH/cyperus-alternifolius.jpg</t>
   </si>
   <si>
     <t>1 - 1.2 m</t>
@@ -1414,6 +1414,9 @@
     <t>https://i.postimg.cc/KzM2QdvT/Caesalpinia-pulcherrima.jpg</t>
   </si>
   <si>
+    <t>Location type</t>
+  </si>
+  <si>
     <t>Location number</t>
   </si>
   <si>
@@ -1423,6 +1426,9 @@
     <t>Quantity</t>
   </si>
   <si>
+    <t>Building</t>
+  </si>
+  <si>
     <t>S13</t>
   </si>
   <si>
@@ -1547,19 +1553,13 @@
   </si>
   <si>
     <t>Gate 3-S55</t>
-  </si>
-  <si>
-    <t>Location type</t>
-  </si>
-  <si>
-    <t>Building</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2059,37 +2059,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F43C3B61-471E-4868-9D01-BC7FF88A37C8}">
   <dimension ref="A1:U186"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D62" sqref="D62"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="4"/>
-    <col min="2" max="2" width="32.453125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="23.1796875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="12.453125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="47.81640625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="17.7265625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="15.26953125" style="4" customWidth="1"/>
-    <col min="8" max="8" width="16.81640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.1796875" style="4" customWidth="1"/>
-    <col min="10" max="10" width="12.453125" style="4" customWidth="1"/>
-    <col min="11" max="11" width="14.54296875" style="4" customWidth="1"/>
-    <col min="12" max="13" width="9.1796875" style="4"/>
-    <col min="14" max="14" width="14.1796875" style="4" customWidth="1"/>
-    <col min="15" max="15" width="11.7265625" style="4" customWidth="1"/>
-    <col min="16" max="16" width="16.26953125" style="4" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.453125" style="4" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.7265625" style="4" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="21.1796875" style="4" customWidth="1"/>
-    <col min="20" max="20" width="27.26953125" style="4" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="33.7265625" style="4" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="9.1796875" style="4"/>
+    <col min="1" max="1" width="9.140625" style="4"/>
+    <col min="2" max="2" width="32.42578125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="47.85546875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" style="4" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.140625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" style="4" customWidth="1"/>
+    <col min="12" max="13" width="9.140625" style="4"/>
+    <col min="14" max="14" width="14.140625" style="4" customWidth="1"/>
+    <col min="15" max="15" width="11.7109375" style="4" customWidth="1"/>
+    <col min="16" max="16" width="16.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21.140625" style="4" customWidth="1"/>
+    <col min="20" max="20" width="27.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="33.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" ht="14.45">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2154,7 +2154,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" ht="14.45">
       <c r="A2" s="4" t="s">
         <v>21</v>
       </c>
@@ -2219,7 +2219,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:21" ht="14.45">
       <c r="A3" s="4" t="s">
         <v>37</v>
       </c>
@@ -2284,7 +2284,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:21" ht="14.45">
       <c r="A4" s="4" t="s">
         <v>49</v>
       </c>
@@ -2349,7 +2349,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:21" ht="14.45">
       <c r="A5" s="4" t="s">
         <v>58</v>
       </c>
@@ -2414,7 +2414,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:21" ht="14.45">
       <c r="A6" s="4" t="s">
         <v>66</v>
       </c>
@@ -2479,7 +2479,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:21" ht="14.45">
       <c r="A7" s="4" t="s">
         <v>75</v>
       </c>
@@ -2544,7 +2544,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:21" ht="14.45">
       <c r="A8" s="4" t="s">
         <v>82</v>
       </c>
@@ -2609,7 +2609,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:21" ht="14.45">
       <c r="A9" s="4" t="s">
         <v>92</v>
       </c>
@@ -2674,7 +2674,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:21" ht="14.45">
       <c r="A10" s="4" t="s">
         <v>97</v>
       </c>
@@ -2739,7 +2739,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:21" ht="14.45">
       <c r="A11" s="4" t="s">
         <v>104</v>
       </c>
@@ -2804,7 +2804,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:21" ht="14.45">
       <c r="A12" s="4" t="s">
         <v>111</v>
       </c>
@@ -2869,7 +2869,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:21" ht="14.45">
       <c r="A13" s="4" t="s">
         <v>115</v>
       </c>
@@ -2934,7 +2934,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:21" ht="14.45">
       <c r="A14" s="4" t="s">
         <v>122</v>
       </c>
@@ -2999,7 +2999,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:21" ht="14.45">
       <c r="A15" s="4" t="s">
         <v>129</v>
       </c>
@@ -3064,7 +3064,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:21" ht="15.75">
       <c r="A16" s="4" t="s">
         <v>136</v>
       </c>
@@ -3129,7 +3129,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="17" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:21" ht="14.45">
       <c r="A17" s="4" t="s">
         <v>143</v>
       </c>
@@ -3194,7 +3194,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="18" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:21" ht="14.45">
       <c r="A18" s="4" t="s">
         <v>150</v>
       </c>
@@ -3259,7 +3259,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="19" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:21" ht="14.45">
       <c r="A19" s="4" t="s">
         <v>159</v>
       </c>
@@ -3324,7 +3324,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="20" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:21" ht="14.45">
       <c r="A20" s="4" t="s">
         <v>167</v>
       </c>
@@ -3389,7 +3389,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="21" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:21" ht="14.45">
       <c r="A21" s="4" t="s">
         <v>175</v>
       </c>
@@ -3454,7 +3454,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="22" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:21" ht="14.45">
       <c r="A22" s="4" t="s">
         <v>183</v>
       </c>
@@ -3519,7 +3519,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:21" ht="14.45">
       <c r="A23" s="4" t="s">
         <v>192</v>
       </c>
@@ -3584,7 +3584,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="24" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:21" ht="14.45">
       <c r="A24" s="4" t="s">
         <v>198</v>
       </c>
@@ -3649,7 +3649,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="25" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:21" ht="14.45">
       <c r="A25" s="4" t="s">
         <v>206</v>
       </c>
@@ -3714,7 +3714,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="26" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:21" ht="14.45">
       <c r="A26" s="4" t="s">
         <v>214</v>
       </c>
@@ -3779,7 +3779,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="27" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:21" ht="14.45">
       <c r="A27" s="4" t="s">
         <v>221</v>
       </c>
@@ -3844,7 +3844,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="28" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:21" ht="14.45">
       <c r="A28" s="4" t="s">
         <v>228</v>
       </c>
@@ -3909,7 +3909,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="29" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:21" ht="14.45">
       <c r="A29" s="4" t="s">
         <v>236</v>
       </c>
@@ -3974,7 +3974,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="30" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:21" ht="14.45">
       <c r="A30" s="4" t="s">
         <v>242</v>
       </c>
@@ -4039,7 +4039,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="31" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:21" ht="14.45">
       <c r="A31" s="4" t="s">
         <v>250</v>
       </c>
@@ -4104,7 +4104,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="32" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:21" ht="15.75" customHeight="1">
       <c r="A32" s="4" t="s">
         <v>257</v>
       </c>
@@ -4169,7 +4169,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="33" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:21" ht="14.45">
       <c r="A33" s="4" t="s">
         <v>265</v>
       </c>
@@ -4234,7 +4234,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="34" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:21" ht="14.45">
       <c r="A34" s="4" t="s">
         <v>271</v>
       </c>
@@ -4299,7 +4299,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="35" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:21" ht="14.45">
       <c r="A35" s="4" t="s">
         <v>277</v>
       </c>
@@ -4364,7 +4364,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="36" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:21" ht="14.45">
       <c r="A36" s="4" t="s">
         <v>283</v>
       </c>
@@ -4429,7 +4429,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="37" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:21" ht="14.45">
       <c r="A37" s="4" t="s">
         <v>290</v>
       </c>
@@ -4494,7 +4494,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="38" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:21" ht="14.45">
       <c r="A38" s="4" t="s">
         <v>295</v>
       </c>
@@ -4559,7 +4559,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="39" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:21" ht="14.45">
       <c r="A39" s="4" t="s">
         <v>301</v>
       </c>
@@ -4624,7 +4624,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="40" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:21" ht="14.45">
       <c r="A40" s="4" t="s">
         <v>306</v>
       </c>
@@ -4689,7 +4689,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="41" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:21" ht="14.45">
       <c r="A41" s="4" t="s">
         <v>313</v>
       </c>
@@ -4754,7 +4754,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="42" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:21" ht="14.45">
       <c r="A42" s="4" t="s">
         <v>321</v>
       </c>
@@ -4819,7 +4819,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="43" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:21" ht="14.45">
       <c r="A43" s="4" t="s">
         <v>327</v>
       </c>
@@ -4884,7 +4884,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="44" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:21" ht="14.45">
       <c r="A44" s="4" t="s">
         <v>333</v>
       </c>
@@ -4949,7 +4949,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="45" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:21" ht="14.45">
       <c r="A45" s="4" t="s">
         <v>338</v>
       </c>
@@ -5014,7 +5014,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="46" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:21" ht="14.45">
       <c r="A46" s="4" t="s">
         <v>342</v>
       </c>
@@ -5079,7 +5079,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="47" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:21" ht="14.45">
       <c r="A47" s="4" t="s">
         <v>349</v>
       </c>
@@ -5144,7 +5144,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="48" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:21" ht="14.45">
       <c r="A48" s="4" t="s">
         <v>356</v>
       </c>
@@ -5209,7 +5209,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="49" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:21" ht="14.45">
       <c r="A49" s="4" t="s">
         <v>364</v>
       </c>
@@ -5274,7 +5274,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="50" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:21" ht="14.45">
       <c r="A50" s="4" t="s">
         <v>371</v>
       </c>
@@ -5339,7 +5339,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="51" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:21" ht="14.45">
       <c r="A51" s="4" t="s">
         <v>377</v>
       </c>
@@ -5404,7 +5404,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="52" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:21" ht="14.45">
       <c r="A52" s="4" t="s">
         <v>384</v>
       </c>
@@ -5469,7 +5469,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="53" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:21" ht="14.45">
       <c r="A53" s="4" t="s">
         <v>390</v>
       </c>
@@ -5534,7 +5534,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="54" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:21" ht="14.45">
       <c r="A54" s="4" t="s">
         <v>398</v>
       </c>
@@ -5599,7 +5599,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="55" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:21" ht="14.45">
       <c r="A55" s="4" t="s">
         <v>405</v>
       </c>
@@ -5664,7 +5664,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="56" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:21" ht="14.45">
       <c r="A56" s="4" t="s">
         <v>410</v>
       </c>
@@ -5729,7 +5729,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="57" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:21" ht="14.45">
       <c r="A57" s="4" t="s">
         <v>418</v>
       </c>
@@ -5794,7 +5794,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="58" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:21" ht="14.45">
       <c r="A58" s="25" t="s">
         <v>425</v>
       </c>
@@ -5859,7 +5859,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="59" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:21" ht="14.45">
       <c r="A59" s="25" t="s">
         <v>432</v>
       </c>
@@ -5924,7 +5924,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="60" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:21" ht="14.45">
       <c r="A60" s="25" t="s">
         <v>439</v>
       </c>
@@ -5989,7 +5989,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="61" spans="1:21" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:21" ht="14.45" customHeight="1">
       <c r="A61" s="24" t="s">
         <v>446</v>
       </c>
@@ -6054,7 +6054,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="62" spans="1:21" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:21" ht="14.45" customHeight="1">
       <c r="A62" s="25" t="s">
         <v>453</v>
       </c>
@@ -6119,130 +6119,130 @@
         <v>452</v>
       </c>
     </row>
-    <row r="63" spans="1:21" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="64" spans="1:21" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="65" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="66" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="67" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="68" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="69" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="70" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="71" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="72" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="73" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="74" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="75" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="76" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="77" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="78" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="79" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="80" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="81" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="82" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="83" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="84" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="85" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="86" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="87" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="88" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="89" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="90" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="91" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="92" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="93" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="94" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="95" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="96" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="97" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="98" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="99" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="100" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="101" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="102" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="103" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="104" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="105" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="106" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="107" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="108" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="109" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="110" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="111" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="112" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="113" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="114" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="115" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="116" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="117" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="118" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="119" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="120" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="121" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="122" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="123" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="124" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="125" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="126" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="127" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="128" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="129" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="130" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="131" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="132" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="133" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="134" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="135" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="136" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="137" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="138" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="139" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="140" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="141" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="142" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="143" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="144" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="145" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="146" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="147" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="148" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="149" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="150" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="151" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="152" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="153" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="154" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="155" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="156" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="157" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="158" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="159" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="160" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="161" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="162" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="163" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="164" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="165" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="166" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="167" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="168" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="169" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="170" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="171" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="172" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="173" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="174" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="175" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="176" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="177" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="178" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="179" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="180" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="181" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="182" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="183" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="184" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="185" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="186" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="63" spans="1:21" ht="14.45"/>
+    <row r="64" spans="1:21" ht="14.45"/>
+    <row r="65" ht="14.45"/>
+    <row r="66" ht="14.45"/>
+    <row r="67" ht="14.45"/>
+    <row r="68" ht="14.45"/>
+    <row r="69" ht="14.45"/>
+    <row r="70" ht="14.45"/>
+    <row r="71" ht="14.45"/>
+    <row r="72" ht="14.45"/>
+    <row r="73" ht="14.45"/>
+    <row r="74" ht="14.45"/>
+    <row r="75" ht="14.45"/>
+    <row r="76" ht="14.45"/>
+    <row r="77" ht="14.45"/>
+    <row r="78" ht="14.45"/>
+    <row r="79" ht="14.45"/>
+    <row r="80" ht="14.45"/>
+    <row r="81" ht="14.45"/>
+    <row r="82" ht="14.45"/>
+    <row r="83" ht="14.45"/>
+    <row r="84" ht="14.45"/>
+    <row r="85" ht="14.45"/>
+    <row r="86" ht="14.45"/>
+    <row r="87" ht="14.45"/>
+    <row r="88" ht="14.45"/>
+    <row r="89" ht="14.45"/>
+    <row r="90" ht="14.45"/>
+    <row r="91" ht="14.45"/>
+    <row r="92" ht="14.45"/>
+    <row r="93" ht="14.45"/>
+    <row r="94" ht="14.45"/>
+    <row r="95" ht="14.45"/>
+    <row r="96" ht="14.45"/>
+    <row r="97" ht="14.45"/>
+    <row r="98" ht="14.45"/>
+    <row r="99" ht="14.45"/>
+    <row r="100" ht="14.45"/>
+    <row r="101" ht="14.45"/>
+    <row r="102" ht="14.45"/>
+    <row r="103" ht="14.45"/>
+    <row r="104" ht="14.45"/>
+    <row r="105" ht="14.45"/>
+    <row r="106" ht="14.45"/>
+    <row r="107" ht="14.45"/>
+    <row r="108" ht="14.45"/>
+    <row r="109" ht="14.45"/>
+    <row r="110" ht="14.45"/>
+    <row r="111" ht="14.45"/>
+    <row r="112" ht="14.45"/>
+    <row r="113" ht="14.45"/>
+    <row r="114" ht="14.45"/>
+    <row r="115" ht="14.45"/>
+    <row r="116" ht="14.45"/>
+    <row r="117" ht="14.45"/>
+    <row r="118" ht="14.45"/>
+    <row r="119" ht="14.45"/>
+    <row r="120" ht="14.45"/>
+    <row r="121" ht="14.45"/>
+    <row r="122" ht="14.45"/>
+    <row r="123" ht="14.45"/>
+    <row r="124" ht="14.45"/>
+    <row r="125" ht="14.45"/>
+    <row r="126" ht="14.45"/>
+    <row r="127" ht="14.45"/>
+    <row r="128" ht="14.45"/>
+    <row r="129" ht="14.45"/>
+    <row r="130" ht="14.45"/>
+    <row r="131" ht="14.45"/>
+    <row r="132" ht="14.45"/>
+    <row r="133" ht="14.45"/>
+    <row r="134" ht="14.45"/>
+    <row r="135" ht="14.45"/>
+    <row r="136" ht="14.45"/>
+    <row r="137" ht="14.45"/>
+    <row r="138" ht="14.45"/>
+    <row r="139" ht="14.45"/>
+    <row r="140" ht="14.45"/>
+    <row r="141" ht="14.45"/>
+    <row r="142" ht="14.45"/>
+    <row r="143" ht="14.45"/>
+    <row r="144" ht="14.45"/>
+    <row r="145" ht="14.45"/>
+    <row r="146" ht="14.45"/>
+    <row r="147" ht="14.45"/>
+    <row r="148" ht="14.45"/>
+    <row r="149" ht="14.45"/>
+    <row r="150" ht="14.45"/>
+    <row r="151" ht="14.45"/>
+    <row r="152" ht="14.45"/>
+    <row r="153" ht="14.45"/>
+    <row r="154" ht="14.45"/>
+    <row r="155" ht="14.45"/>
+    <row r="156" ht="14.45"/>
+    <row r="157" ht="14.45"/>
+    <row r="158" ht="14.45"/>
+    <row r="159" ht="14.45"/>
+    <row r="160" ht="14.45"/>
+    <row r="161" ht="14.45"/>
+    <row r="162" ht="14.45"/>
+    <row r="163" ht="14.45"/>
+    <row r="164" ht="14.45"/>
+    <row r="165" ht="14.45"/>
+    <row r="166" ht="14.45"/>
+    <row r="167" ht="14.45"/>
+    <row r="168" ht="14.45"/>
+    <row r="169" ht="14.45"/>
+    <row r="170" ht="14.45"/>
+    <row r="171" ht="14.45"/>
+    <row r="172" ht="14.45"/>
+    <row r="173" ht="14.45"/>
+    <row r="174" ht="14.45"/>
+    <row r="175" ht="14.45"/>
+    <row r="176" ht="14.45"/>
+    <row r="177" ht="14.45"/>
+    <row r="178" ht="14.45"/>
+    <row r="179" ht="14.45"/>
+    <row r="180" ht="14.45"/>
+    <row r="181" ht="14.45"/>
+    <row r="182" ht="14.45"/>
+    <row r="183" ht="14.45"/>
+    <row r="184" ht="14.45"/>
+    <row r="185" ht="14.45"/>
+    <row r="186" ht="14.45"/>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:U45">
     <sortCondition ref="A2:A45"/>
@@ -6415,902 +6415,902 @@
   </sheetPr>
   <dimension ref="A1:G163"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="17.54296875" customWidth="1"/>
-    <col min="3" max="3" width="50.453125" customWidth="1"/>
-    <col min="4" max="4" width="18.1796875" customWidth="1"/>
-    <col min="5" max="5" width="16.7265625" customWidth="1"/>
-    <col min="6" max="6" width="34.26953125" style="11" customWidth="1"/>
-    <col min="7" max="7" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="17.5703125" customWidth="1"/>
+    <col min="3" max="3" width="50.42578125" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="6" max="6" width="34.28515625" style="11" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="20" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" s="20" customFormat="1" ht="26.25" customHeight="1">
       <c r="A1" s="20" t="s">
-        <v>502</v>
+        <v>457</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1">
       <c r="A2" s="20" t="s">
-        <v>503</v>
+        <v>461</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="E2" s="21"/>
       <c r="F2" s="21"/>
     </row>
-    <row r="3" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1">
       <c r="A3" s="20" t="s">
-        <v>503</v>
+        <v>461</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="E3" s="22"/>
       <c r="F3" s="21"/>
     </row>
-    <row r="4" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1">
       <c r="A4" s="20" t="s">
-        <v>503</v>
+        <v>461</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="E4" s="22"/>
       <c r="F4" s="21"/>
     </row>
-    <row r="5" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1">
       <c r="A5" s="20" t="s">
-        <v>503</v>
+        <v>461</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="C5" s="21"/>
       <c r="E5" s="21"/>
       <c r="F5" s="21"/>
     </row>
-    <row r="6" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1">
       <c r="A6" s="20" t="s">
-        <v>503</v>
+        <v>461</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="E6" s="21"/>
       <c r="F6" s="21"/>
     </row>
-    <row r="7" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1">
       <c r="A7" s="20" t="s">
-        <v>503</v>
+        <v>461</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E7" s="22"/>
       <c r="F7" s="21"/>
     </row>
-    <row r="8" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1">
       <c r="A8" s="20" t="s">
-        <v>503</v>
+        <v>461</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="E8" s="22"/>
       <c r="F8" s="21"/>
     </row>
-    <row r="9" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1">
       <c r="A9" s="20" t="s">
-        <v>503</v>
+        <v>461</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="E9" s="21"/>
       <c r="F9" s="21"/>
     </row>
-    <row r="10" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1">
       <c r="A10" s="20" t="s">
-        <v>503</v>
+        <v>461</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="C10" s="21"/>
       <c r="E10" s="21"/>
       <c r="F10" s="21"/>
     </row>
-    <row r="11" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1">
       <c r="A11" s="20" t="s">
-        <v>503</v>
+        <v>461</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="E11" s="22"/>
       <c r="F11" s="21"/>
     </row>
-    <row r="12" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1">
       <c r="A12" s="20" t="s">
-        <v>503</v>
+        <v>461</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="C12" s="23"/>
       <c r="E12" s="22"/>
       <c r="F12" s="21"/>
     </row>
-    <row r="13" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1">
       <c r="A13" s="20" t="s">
-        <v>503</v>
+        <v>461</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="E13" s="21"/>
       <c r="F13" s="21"/>
     </row>
-    <row r="14" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1">
       <c r="A14" s="20" t="s">
-        <v>503</v>
+        <v>461</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="E14" s="22"/>
       <c r="F14" s="21"/>
     </row>
-    <row r="15" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1">
       <c r="A15" s="20" t="s">
-        <v>503</v>
+        <v>461</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="E15" s="22"/>
       <c r="F15" s="21"/>
     </row>
-    <row r="16" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1">
       <c r="A16" s="20" t="s">
-        <v>503</v>
+        <v>461</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="E16" s="21"/>
       <c r="F16" s="21"/>
     </row>
-    <row r="17" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1">
       <c r="A17" s="20" t="s">
-        <v>503</v>
+        <v>461</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="C17" s="21"/>
       <c r="E17" s="21"/>
       <c r="F17" s="21"/>
     </row>
-    <row r="18" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1">
       <c r="A18" s="20" t="s">
-        <v>503</v>
+        <v>461</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="E18" s="21"/>
       <c r="F18" s="21"/>
     </row>
-    <row r="19" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1">
       <c r="A19" s="20" t="s">
-        <v>503</v>
+        <v>461</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="E19" s="21"/>
       <c r="F19" s="21"/>
     </row>
-    <row r="20" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1">
       <c r="A20" s="20" t="s">
-        <v>503</v>
+        <v>461</v>
       </c>
       <c r="B20" s="20" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="E20" s="21"/>
       <c r="F20" s="21"/>
     </row>
-    <row r="21" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1">
       <c r="A21" s="20" t="s">
-        <v>503</v>
+        <v>461</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="E21" s="21"/>
       <c r="F21" s="21"/>
     </row>
-    <row r="22" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1">
       <c r="A22" s="20" t="s">
-        <v>503</v>
+        <v>461</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="E22" s="21"/>
       <c r="F22" s="21"/>
     </row>
-    <row r="23" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1">
       <c r="A23" s="20" t="s">
-        <v>503</v>
+        <v>461</v>
       </c>
       <c r="B23" s="20" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="E23" s="21"/>
       <c r="F23" s="21"/>
     </row>
-    <row r="24" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1">
       <c r="A24" s="20" t="s">
-        <v>503</v>
+        <v>461</v>
       </c>
       <c r="B24" s="20" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="E24" s="21"/>
       <c r="F24" s="21"/>
     </row>
-    <row r="25" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1">
       <c r="A25" s="20" t="s">
-        <v>503</v>
+        <v>461</v>
       </c>
       <c r="B25" s="20" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="E25" s="21"/>
       <c r="F25" s="21"/>
     </row>
-    <row r="26" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1">
       <c r="A26" s="20" t="s">
-        <v>503</v>
+        <v>461</v>
       </c>
       <c r="B26" s="20" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="E26" s="21"/>
       <c r="F26" s="21"/>
     </row>
-    <row r="27" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1">
       <c r="A27" s="20" t="s">
-        <v>503</v>
+        <v>461</v>
       </c>
       <c r="B27" s="20" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="E27" s="21"/>
       <c r="F27" s="21"/>
     </row>
-    <row r="28" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1">
       <c r="A28" s="20" t="s">
-        <v>503</v>
+        <v>461</v>
       </c>
       <c r="B28" s="20" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="E28" s="21"/>
       <c r="F28" s="21"/>
     </row>
-    <row r="29" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1">
       <c r="A29" s="20" t="s">
-        <v>503</v>
+        <v>461</v>
       </c>
       <c r="B29" s="20" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="E29" s="21"/>
       <c r="F29" s="21"/>
     </row>
-    <row r="30" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1">
       <c r="A30" s="20" t="s">
-        <v>503</v>
+        <v>461</v>
       </c>
       <c r="B30" s="20" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="E30" s="21"/>
       <c r="F30" s="21"/>
     </row>
-    <row r="31" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1">
       <c r="A31" s="20" t="s">
-        <v>503</v>
+        <v>461</v>
       </c>
       <c r="B31" s="20" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="E31" s="21"/>
       <c r="F31" s="21"/>
     </row>
-    <row r="32" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" s="20" customFormat="1" ht="50.25" customHeight="1">
       <c r="A32" s="20" t="s">
-        <v>503</v>
+        <v>461</v>
       </c>
       <c r="B32" s="20" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="E32" s="21"/>
       <c r="F32" s="21"/>
     </row>
-    <row r="33" spans="1:7" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" s="20" customFormat="1" ht="50.25" customHeight="1">
       <c r="A33" s="20" t="s">
-        <v>503</v>
+        <v>461</v>
       </c>
       <c r="B33" s="20" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="C33" s="21"/>
       <c r="E33" s="21"/>
       <c r="F33" s="21"/>
     </row>
-    <row r="34" spans="1:7" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" s="20" customFormat="1" ht="50.25" customHeight="1">
       <c r="A34" s="20" t="s">
-        <v>503</v>
+        <v>461</v>
       </c>
       <c r="B34" s="20" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="E34" s="21"/>
       <c r="F34" s="21"/>
     </row>
-    <row r="35" spans="1:7" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" s="20" customFormat="1" ht="50.25" customHeight="1">
       <c r="A35" s="20" t="s">
-        <v>503</v>
+        <v>461</v>
       </c>
       <c r="B35" s="20" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="E35" s="21"/>
       <c r="F35" s="21"/>
     </row>
-    <row r="36" spans="1:7" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" s="20" customFormat="1" ht="50.25" customHeight="1">
       <c r="A36" s="20" t="s">
-        <v>503</v>
+        <v>461</v>
       </c>
       <c r="B36" s="20" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c r="E36" s="21"/>
       <c r="F36" s="21"/>
     </row>
-    <row r="37" spans="1:7" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" s="20" customFormat="1" ht="50.25" customHeight="1">
       <c r="A37" s="20" t="s">
-        <v>503</v>
+        <v>461</v>
       </c>
       <c r="B37" s="20" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="E37" s="21"/>
       <c r="F37" s="21"/>
     </row>
-    <row r="38" spans="1:7" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" s="20" customFormat="1" ht="50.25" customHeight="1">
       <c r="A38" s="20" t="s">
-        <v>503</v>
+        <v>461</v>
       </c>
       <c r="B38" s="20" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="E38" s="21"/>
       <c r="F38" s="21"/>
     </row>
-    <row r="39" spans="1:7" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" s="20" customFormat="1" ht="50.25" customHeight="1">
       <c r="A39" s="20" t="s">
-        <v>503</v>
+        <v>461</v>
       </c>
       <c r="B39" s="20" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="E39" s="21"/>
       <c r="F39" s="21"/>
     </row>
-    <row r="40" spans="1:7" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" s="20" customFormat="1" ht="50.25" customHeight="1">
       <c r="A40" s="20" t="s">
-        <v>503</v>
+        <v>461</v>
       </c>
       <c r="B40" s="20" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="E40" s="21"/>
       <c r="F40" s="21"/>
     </row>
-    <row r="41" spans="1:7" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" s="20" customFormat="1" ht="50.25" customHeight="1">
       <c r="A41" s="20" t="s">
-        <v>503</v>
+        <v>461</v>
       </c>
       <c r="B41" s="20" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="E41" s="21"/>
       <c r="F41" s="21"/>
     </row>
-    <row r="42" spans="1:7" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" s="20" customFormat="1" ht="50.25" customHeight="1">
       <c r="A42" s="20" t="s">
-        <v>503</v>
+        <v>461</v>
       </c>
       <c r="B42" s="20" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="E42" s="21"/>
       <c r="F42" s="21"/>
     </row>
-    <row r="43" spans="1:7" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" s="20" customFormat="1" ht="50.25" customHeight="1">
       <c r="A43" s="20" t="s">
-        <v>503</v>
+        <v>461</v>
       </c>
       <c r="B43" s="20" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c r="E43" s="21"/>
       <c r="F43" s="21"/>
     </row>
-    <row r="44" spans="1:7" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" s="20" customFormat="1" ht="50.25" customHeight="1">
       <c r="A44" s="20" t="s">
-        <v>503</v>
+        <v>461</v>
       </c>
       <c r="B44" s="20" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="E44" s="21"/>
       <c r="F44" s="21"/>
     </row>
-    <row r="45" spans="1:7" s="20" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" s="20" customFormat="1" ht="50.25" customHeight="1">
       <c r="A45" s="20" t="s">
+        <v>461</v>
+      </c>
+      <c r="B45" s="20" t="s">
         <v>503</v>
-      </c>
-      <c r="B45" s="20" t="s">
-        <v>501</v>
       </c>
       <c r="E45" s="21"/>
       <c r="F45" s="21"/>
     </row>
-    <row r="46" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" ht="14.45">
       <c r="A46" s="20"/>
       <c r="E46" s="16"/>
       <c r="F46" s="17"/>
       <c r="G46" s="1"/>
     </row>
-    <row r="47" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" ht="14.45">
       <c r="E47" s="16"/>
       <c r="F47" s="17"/>
       <c r="G47" s="1"/>
     </row>
-    <row r="48" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" ht="14.45">
       <c r="F48" s="18"/>
       <c r="G48" s="1"/>
     </row>
-    <row r="49" spans="6:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="6:7" ht="14.45">
       <c r="F49" s="18"/>
       <c r="G49" s="1"/>
     </row>
-    <row r="50" spans="6:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="50" spans="6:7" ht="14.45">
       <c r="F50" s="18"/>
       <c r="G50" s="1"/>
     </row>
-    <row r="51" spans="6:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="51" spans="6:7" ht="14.45">
       <c r="F51" s="18"/>
       <c r="G51" s="1"/>
     </row>
-    <row r="52" spans="6:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="52" spans="6:7" ht="14.45">
       <c r="F52" s="18"/>
       <c r="G52" s="1"/>
     </row>
-    <row r="53" spans="6:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="53" spans="6:7" ht="14.45">
       <c r="F53" s="18"/>
       <c r="G53" s="1"/>
     </row>
-    <row r="54" spans="6:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="54" spans="6:7" ht="14.45">
       <c r="F54" s="18"/>
       <c r="G54" s="1"/>
     </row>
-    <row r="55" spans="6:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="55" spans="6:7" ht="14.45">
       <c r="F55" s="18"/>
       <c r="G55" s="1"/>
     </row>
-    <row r="56" spans="6:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="56" spans="6:7" ht="14.45">
       <c r="F56" s="18"/>
       <c r="G56" s="1"/>
     </row>
-    <row r="57" spans="6:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="57" spans="6:7" ht="14.45">
       <c r="F57" s="18"/>
       <c r="G57" s="1"/>
     </row>
-    <row r="58" spans="6:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="58" spans="6:7" ht="14.45">
       <c r="F58" s="18"/>
       <c r="G58" s="1"/>
     </row>
-    <row r="59" spans="6:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="59" spans="6:7" ht="14.45">
       <c r="F59" s="18"/>
       <c r="G59" s="1"/>
     </row>
-    <row r="60" spans="6:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="60" spans="6:7" ht="14.45">
       <c r="F60" s="18"/>
       <c r="G60" s="1"/>
     </row>
-    <row r="61" spans="6:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="61" spans="6:7" ht="14.45">
       <c r="F61" s="18"/>
       <c r="G61" s="1"/>
     </row>
-    <row r="62" spans="6:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="62" spans="6:7" ht="14.45">
       <c r="F62" s="18"/>
       <c r="G62" s="1"/>
     </row>
-    <row r="63" spans="6:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="63" spans="6:7" ht="14.45">
       <c r="F63" s="18"/>
       <c r="G63" s="1"/>
     </row>
-    <row r="64" spans="6:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="64" spans="6:7" ht="14.45">
       <c r="F64" s="18"/>
       <c r="G64" s="1"/>
     </row>
-    <row r="65" spans="6:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="65" spans="6:7" ht="14.45">
       <c r="F65" s="18"/>
       <c r="G65" s="1"/>
     </row>
-    <row r="66" spans="6:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="66" spans="6:7" ht="14.45">
       <c r="F66" s="18"/>
       <c r="G66" s="1"/>
     </row>
-    <row r="67" spans="6:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="67" spans="6:7" ht="14.45">
       <c r="F67" s="18"/>
       <c r="G67" s="1"/>
     </row>
-    <row r="68" spans="6:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="68" spans="6:7" ht="14.45">
       <c r="F68" s="18"/>
       <c r="G68" s="1"/>
     </row>
-    <row r="69" spans="6:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="69" spans="6:7" ht="14.45">
       <c r="F69" s="18"/>
       <c r="G69" s="1"/>
     </row>
-    <row r="70" spans="6:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="70" spans="6:7" ht="14.45">
       <c r="F70" s="18"/>
       <c r="G70" s="1"/>
     </row>
-    <row r="71" spans="6:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="71" spans="6:7" ht="14.45">
       <c r="F71" s="18"/>
       <c r="G71" s="1"/>
     </row>
-    <row r="72" spans="6:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="72" spans="6:7" ht="14.45">
       <c r="F72" s="18"/>
       <c r="G72" s="1"/>
     </row>
-    <row r="73" spans="6:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="73" spans="6:7" ht="14.45">
       <c r="F73" s="18"/>
       <c r="G73" s="1"/>
     </row>
-    <row r="74" spans="6:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="74" spans="6:7" ht="14.45">
       <c r="G74" s="1"/>
     </row>
-    <row r="75" spans="6:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="75" spans="6:7" ht="14.45">
       <c r="G75" s="1"/>
     </row>
-    <row r="76" spans="6:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="76" spans="6:7" ht="14.45">
       <c r="G76" s="1"/>
     </row>
-    <row r="77" spans="6:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="77" spans="6:7" ht="14.45">
       <c r="G77" s="1"/>
     </row>
-    <row r="78" spans="6:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="78" spans="6:7" ht="14.45">
       <c r="G78" s="1"/>
     </row>
-    <row r="79" spans="6:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="79" spans="6:7" ht="14.45">
       <c r="G79" s="1"/>
     </row>
-    <row r="80" spans="6:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="80" spans="6:7" ht="14.45">
       <c r="G80" s="1"/>
     </row>
-    <row r="81" spans="6:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="81" spans="6:7" ht="14.45">
       <c r="G81" s="1"/>
     </row>
-    <row r="82" spans="6:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="82" spans="6:7" ht="14.45">
       <c r="G82" s="1"/>
     </row>
-    <row r="83" spans="6:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="83" spans="6:7" ht="14.45">
       <c r="G83" s="1"/>
     </row>
-    <row r="84" spans="6:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="84" spans="6:7" ht="14.45">
       <c r="G84" s="1"/>
     </row>
-    <row r="85" spans="6:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="85" spans="6:7" ht="14.45">
       <c r="G85" s="1"/>
     </row>
-    <row r="86" spans="6:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="86" spans="6:7" ht="14.45">
       <c r="G86" s="1"/>
     </row>
-    <row r="87" spans="6:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="87" spans="6:7" ht="14.45">
       <c r="G87" s="1"/>
     </row>
-    <row r="88" spans="6:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="88" spans="6:7" ht="14.45">
       <c r="G88" s="1"/>
     </row>
-    <row r="89" spans="6:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="89" spans="6:7" ht="14.45">
       <c r="G89" s="1"/>
     </row>
-    <row r="90" spans="6:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="90" spans="6:7" ht="14.45">
       <c r="G90" s="1"/>
     </row>
-    <row r="91" spans="6:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="91" spans="6:7" ht="14.45">
       <c r="G91" s="1"/>
     </row>
-    <row r="92" spans="6:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="92" spans="6:7" ht="14.45">
       <c r="G92" s="1"/>
     </row>
-    <row r="93" spans="6:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="93" spans="6:7" ht="14.45">
       <c r="G93" s="1"/>
     </row>
-    <row r="94" spans="6:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="94" spans="6:7" ht="15.6">
       <c r="F94" s="19"/>
       <c r="G94" s="1"/>
     </row>
-    <row r="95" spans="6:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="95" spans="6:7" ht="15.6">
       <c r="F95" s="19"/>
       <c r="G95" s="1"/>
     </row>
-    <row r="96" spans="6:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="96" spans="6:7" ht="15.6">
       <c r="F96" s="19"/>
       <c r="G96" s="1"/>
     </row>
-    <row r="97" spans="6:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="97" spans="6:7" ht="15.6">
       <c r="F97" s="19"/>
       <c r="G97" s="1"/>
     </row>
-    <row r="98" spans="6:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="98" spans="6:7" ht="15.6">
       <c r="F98" s="19"/>
       <c r="G98" s="1"/>
     </row>
-    <row r="99" spans="6:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="99" spans="6:7" ht="15.6">
       <c r="F99" s="19"/>
       <c r="G99" s="1"/>
     </row>
-    <row r="100" spans="6:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="100" spans="6:7" ht="15.6">
       <c r="F100" s="19"/>
       <c r="G100" s="1"/>
     </row>
-    <row r="101" spans="6:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="101" spans="6:7" ht="15.6">
       <c r="F101" s="19"/>
       <c r="G101" s="1"/>
     </row>
-    <row r="102" spans="6:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="102" spans="6:7" ht="15.6">
       <c r="F102" s="19"/>
       <c r="G102" s="1"/>
     </row>
-    <row r="103" spans="6:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="103" spans="6:7" ht="15.6">
       <c r="F103" s="19"/>
       <c r="G103" s="1"/>
     </row>
-    <row r="104" spans="6:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="104" spans="6:7" ht="15.6">
       <c r="F104" s="19"/>
       <c r="G104" s="1"/>
     </row>
-    <row r="105" spans="6:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="105" spans="6:7" ht="15.6">
       <c r="F105" s="19"/>
       <c r="G105" s="1"/>
     </row>
-    <row r="106" spans="6:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="106" spans="6:7" ht="15.6">
       <c r="F106" s="19"/>
       <c r="G106" s="1"/>
     </row>
-    <row r="107" spans="6:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="107" spans="6:7" ht="15.6">
       <c r="F107" s="19"/>
       <c r="G107" s="1"/>
     </row>
-    <row r="108" spans="6:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="108" spans="6:7" ht="15.6">
       <c r="F108" s="19"/>
       <c r="G108" s="1"/>
     </row>
-    <row r="109" spans="6:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="109" spans="6:7" ht="15.6">
       <c r="F109" s="19"/>
       <c r="G109" s="1"/>
     </row>
-    <row r="110" spans="6:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="110" spans="6:7" ht="15.6">
       <c r="F110" s="19"/>
       <c r="G110" s="1"/>
     </row>
-    <row r="111" spans="6:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="111" spans="6:7" ht="15.6">
       <c r="F111" s="19"/>
       <c r="G111" s="1"/>
     </row>
-    <row r="112" spans="6:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="112" spans="6:7" ht="15.6">
       <c r="F112" s="19"/>
       <c r="G112" s="1"/>
     </row>
-    <row r="113" spans="6:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="113" spans="6:7" ht="15.6">
       <c r="F113" s="19"/>
       <c r="G113" s="1"/>
     </row>
-    <row r="114" spans="6:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="114" spans="6:7" ht="14.45">
       <c r="F114" s="18"/>
       <c r="G114" s="1"/>
     </row>
-    <row r="115" spans="6:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="115" spans="6:7" ht="14.45">
       <c r="F115" s="18"/>
       <c r="G115" s="1"/>
     </row>
-    <row r="116" spans="6:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="116" spans="6:7" ht="14.45">
       <c r="F116" s="18"/>
       <c r="G116" s="1"/>
     </row>
-    <row r="117" spans="6:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="117" spans="6:7" ht="14.45">
       <c r="F117" s="18"/>
       <c r="G117" s="1"/>
     </row>
-    <row r="118" spans="6:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="118" spans="6:7" ht="14.45">
       <c r="F118" s="18"/>
       <c r="G118" s="1"/>
     </row>
-    <row r="119" spans="6:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="119" spans="6:7" ht="14.45">
       <c r="F119" s="18"/>
       <c r="G119" s="1"/>
     </row>
-    <row r="120" spans="6:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="120" spans="6:7" ht="14.45">
       <c r="F120" s="18"/>
       <c r="G120" s="1"/>
     </row>
-    <row r="121" spans="6:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="121" spans="6:7" ht="14.45">
       <c r="F121" s="18"/>
       <c r="G121" s="1"/>
     </row>
-    <row r="122" spans="6:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="122" spans="6:7" ht="14.45">
       <c r="F122" s="18"/>
       <c r="G122" s="1"/>
     </row>
-    <row r="123" spans="6:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="123" spans="6:7" ht="14.45">
       <c r="F123" s="18"/>
       <c r="G123" s="1"/>
     </row>
-    <row r="124" spans="6:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="124" spans="6:7" ht="14.45">
       <c r="F124" s="18"/>
       <c r="G124" s="1"/>
     </row>
-    <row r="125" spans="6:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="125" spans="6:7" ht="14.45">
       <c r="F125" s="18"/>
       <c r="G125" s="1"/>
     </row>
-    <row r="126" spans="6:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="126" spans="6:7" ht="14.45">
       <c r="F126" s="18"/>
       <c r="G126" s="1"/>
     </row>
-    <row r="127" spans="6:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="127" spans="6:7" ht="14.45">
       <c r="F127" s="18"/>
       <c r="G127" s="1"/>
     </row>
-    <row r="128" spans="6:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="128" spans="6:7" ht="14.45">
       <c r="F128" s="18"/>
       <c r="G128" s="1"/>
     </row>
-    <row r="129" spans="6:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="129" spans="6:7" ht="14.45">
       <c r="F129" s="18"/>
       <c r="G129" s="1"/>
     </row>
-    <row r="130" spans="6:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="130" spans="6:7" ht="14.45">
       <c r="F130" s="18"/>
       <c r="G130" s="1"/>
     </row>
-    <row r="131" spans="6:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="131" spans="6:7" ht="14.45">
       <c r="F131" s="18"/>
       <c r="G131" s="1"/>
     </row>
-    <row r="132" spans="6:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="132" spans="6:7" ht="14.45">
       <c r="F132" s="18"/>
       <c r="G132" s="1"/>
     </row>
-    <row r="133" spans="6:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="133" spans="6:7" ht="14.45">
       <c r="G133" s="1"/>
     </row>
-    <row r="134" spans="6:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="134" spans="6:7" ht="14.45">
       <c r="G134" s="1"/>
     </row>
-    <row r="135" spans="6:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="135" spans="6:7" ht="14.45">
       <c r="G135" s="1"/>
     </row>
-    <row r="136" spans="6:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="6:7" ht="15" customHeight="1">
       <c r="G136" s="1"/>
     </row>
-    <row r="137" spans="6:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="137" spans="6:7" ht="15" customHeight="1">
       <c r="G137" s="1"/>
     </row>
-    <row r="138" spans="6:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="6:7" ht="15" customHeight="1">
       <c r="G138" s="1"/>
     </row>
-    <row r="139" spans="6:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="6:7" ht="15" customHeight="1">
       <c r="G139" s="1"/>
     </row>
-    <row r="140" spans="6:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="140" spans="6:7" ht="15" customHeight="1">
       <c r="G140" s="1"/>
     </row>
-    <row r="141" spans="6:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="6:7" ht="15" customHeight="1">
       <c r="G141" s="1"/>
     </row>
-    <row r="142" spans="6:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="142" spans="6:7" ht="15" customHeight="1">
       <c r="G142" s="1"/>
     </row>
-    <row r="143" spans="6:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="143" spans="6:7" ht="15" customHeight="1">
       <c r="G143" s="1"/>
     </row>
-    <row r="144" spans="6:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="144" spans="6:7" ht="15" customHeight="1">
       <c r="G144" s="1"/>
     </row>
-    <row r="145" spans="7:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="145" spans="7:7" ht="15" customHeight="1">
       <c r="G145" s="1"/>
     </row>
-    <row r="146" spans="7:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="146" spans="7:7" ht="15" customHeight="1">
       <c r="G146" s="1"/>
     </row>
-    <row r="147" spans="7:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="147" spans="7:7" ht="15" customHeight="1">
       <c r="G147" s="1"/>
     </row>
-    <row r="148" spans="7:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="148" spans="7:7" ht="15" customHeight="1">
       <c r="G148" s="1"/>
     </row>
-    <row r="149" spans="7:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="149" spans="7:7" ht="15" customHeight="1">
       <c r="G149" s="1"/>
     </row>
-    <row r="150" spans="7:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="150" spans="7:7" ht="15" customHeight="1">
       <c r="G150" s="1"/>
     </row>
-    <row r="151" spans="7:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="7:7" ht="15" customHeight="1">
       <c r="G151" s="1"/>
     </row>
-    <row r="152" spans="7:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="152" spans="7:7" ht="15" customHeight="1">
       <c r="G152" s="1"/>
     </row>
-    <row r="153" spans="7:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="153" spans="7:7" ht="15" customHeight="1">
       <c r="G153" s="1"/>
     </row>
-    <row r="154" spans="7:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="154" spans="7:7" ht="15" customHeight="1">
       <c r="G154" s="1"/>
     </row>
-    <row r="155" spans="7:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="155" spans="7:7" ht="15" customHeight="1">
       <c r="G155" s="1"/>
     </row>
-    <row r="156" spans="7:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="156" spans="7:7" ht="15" customHeight="1">
       <c r="G156" s="1"/>
     </row>
-    <row r="157" spans="7:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="157" spans="7:7" ht="15" customHeight="1">
       <c r="G157" s="1"/>
     </row>
-    <row r="158" spans="7:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="158" spans="7:7" ht="15" customHeight="1">
       <c r="G158" s="1"/>
     </row>
-    <row r="159" spans="7:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="159" spans="7:7" ht="15" customHeight="1">
       <c r="G159" s="1"/>
     </row>
-    <row r="160" spans="7:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="160" spans="7:7" ht="15" customHeight="1">
       <c r="G160" s="1"/>
     </row>
-    <row r="161" spans="7:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="161" spans="7:7" ht="15" customHeight="1">
       <c r="G161" s="1"/>
     </row>
-    <row r="162" spans="7:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="162" spans="7:7" ht="15" customHeight="1">
       <c r="G162" s="1"/>
     </row>
-    <row r="163" spans="7:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="163" spans="7:7" ht="15" customHeight="1">
       <c r="G163" s="1"/>
     </row>
   </sheetData>
@@ -7333,6 +7333,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="7855343b-5261-4afc-a17c-d4c130fbaa85" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000D89A625C5B6364BB7302BED22ED65DA" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="05bac8ad6e033965382d52c38353e541">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="7855343b-5261-4afc-a17c-d4c130fbaa85" xmlns:ns4="72f917e0-5d36-43ac-975d-26afa4cf7fc0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="452e5605b09f318b6d66379e79837bd5" ns3:_="" ns4:_="">
     <xsd:import namespace="7855343b-5261-4afc-a17c-d4c130fbaa85"/>
@@ -7579,56 +7596,14 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="7855343b-5261-4afc-a17c-d4c130fbaa85" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56978299-3DC6-451D-A1E5-57FB07C431CC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="7855343b-5261-4afc-a17c-d4c130fbaa85"/>
-    <ds:schemaRef ds:uri="72f917e0-5d36-43ac-975d-26afa4cf7fc0"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BE4A15A-EC2D-4537-B6DC-2F235DBE6314}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BE4A15A-EC2D-4537-B6DC-2F235DBE6314}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F53F9CFB-0E7D-4BF1-9CBE-0D133C6536E4}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F53F9CFB-0E7D-4BF1-9CBE-0D133C6536E4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="7855343b-5261-4afc-a17c-d4c130fbaa85"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56978299-3DC6-451D-A1E5-57FB07C431CC}"/>
 </file>
</xml_diff>